<commit_message>
renaming should be complete documentation update progress
</commit_message>
<xml_diff>
--- a/Documentation/project timeline.xlsx
+++ b/Documentation/project timeline.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C47973E-2C92-49EE-A090-D8F86F5AA9E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Timeline" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
     <definedName name="WindowDays">calcs!$D$29</definedName>
     <definedName name="WindowOffset">calcs!$D$26</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Activity</t>
   </si>
@@ -155,11 +156,17 @@
   <si>
     <t>penultimate writeup</t>
   </si>
+  <si>
+    <t>Ericson's approval to basically do the whole project differently and alone</t>
+  </si>
+  <si>
+    <t>Abandonment</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mmm\ yyyy"/>
   </numFmts>
@@ -347,7 +354,7 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -386,6 +393,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
@@ -458,7 +468,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight8">
-    <tableStyle name="Project Timeline" pivot="0" count="4">
+    <tableStyle name="Project Timeline" pivot="0" count="4" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="3"/>
       <tableStyleElement type="headerRow" dxfId="2"/>
       <tableStyleElement type="firstRowStripe" dxfId="1"/>
@@ -2379,9 +2389,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000002-9B1A-4808-B570-F39EFF2D7B24}"/>
                 </c:ext>
@@ -2422,7 +2430,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -2724,7 +2731,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -3033,7 +3039,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -3342,7 +3347,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -3651,7 +3655,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -4208,7 +4211,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -4557,7 +4559,6 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$E$72</c:f>
@@ -4578,10 +4579,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{B1907344-C67C-4240-A137-18EC31292701}</c15:txfldGUID>
+                      <c15:txfldGUID>{65F84D80-D0F7-48EA-9FEE-93DC87D057CE}</c15:txfldGUID>
                       <c15:f>calcs!$E$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -4600,7 +4600,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$F$72</c:f>
@@ -4621,10 +4620,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{7FB0FE74-DF36-4EF4-BFD2-946BE6AE1E63}</c15:txfldGUID>
+                      <c15:txfldGUID>{A1540CEE-BA27-42C4-916F-5D5AEE343ADE}</c15:txfldGUID>
                       <c15:f>calcs!$F$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -4643,7 +4641,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$G$72</c:f>
@@ -4664,10 +4661,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{EE0F0A06-511C-45CB-9F61-5D92163B6739}</c15:txfldGUID>
+                      <c15:txfldGUID>{CF20AFE9-FF4B-4A99-9981-11021F5CA6F9}</c15:txfldGUID>
                       <c15:f>calcs!$G$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -4686,7 +4682,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$H$72</c:f>
@@ -4707,10 +4702,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{5D2FADB1-825C-4CC5-ABA6-47E75A67B35A}</c15:txfldGUID>
+                      <c15:txfldGUID>{7EC3A0A0-82A9-4474-9D2C-5133620CB130}</c15:txfldGUID>
                       <c15:f>calcs!$H$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -4729,7 +4723,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$I$72</c:f>
@@ -4750,10 +4743,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{351745B9-CE42-4621-9F12-ECFBF4655CF4}</c15:txfldGUID>
+                      <c15:txfldGUID>{4ED5A793-C57E-4365-AAF6-D05473AA3E77}</c15:txfldGUID>
                       <c15:f>calcs!$I$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -4772,7 +4764,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="5"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$J$72</c:f>
@@ -4793,10 +4784,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{DEA4DF36-2C29-47D5-8D93-D4C0394DECA0}</c15:txfldGUID>
+                      <c15:txfldGUID>{184C505B-0653-45A6-BEF4-982C8798BC44}</c15:txfldGUID>
                       <c15:f>calcs!$J$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -4815,7 +4805,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="6"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$K$72</c:f>
@@ -4836,10 +4825,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{F2B2639E-CDB6-410E-8214-4C04125E2A4F}</c15:txfldGUID>
+                      <c15:txfldGUID>{74E52553-E485-49D4-A165-3BF82EB49CAF}</c15:txfldGUID>
                       <c15:f>calcs!$K$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -4858,7 +4846,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="7"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$L$72</c:f>
@@ -4879,10 +4866,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{FEB0FC8F-4FDA-4F05-8F5F-A56F61564655}</c15:txfldGUID>
+                      <c15:txfldGUID>{99EC5A5A-C2EF-4C4D-BF12-3575841B5AF3}</c15:txfldGUID>
                       <c15:f>calcs!$L$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -4901,7 +4887,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="8"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$M$72</c:f>
@@ -4922,10 +4907,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{CC76E3B9-78BD-4358-AA33-5E111CF1FA8F}</c15:txfldGUID>
+                      <c15:txfldGUID>{19002E92-295F-4AEF-8A31-BD9A3AC9A6AE}</c15:txfldGUID>
                       <c15:f>calcs!$M$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -4944,7 +4928,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="9"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$N$72</c:f>
@@ -4965,10 +4948,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{038C26BE-F5D1-4EC9-885A-EF608C67F0AB}</c15:txfldGUID>
+                      <c15:txfldGUID>{2FA7078C-1B11-490E-8828-DFBF3AF582E4}</c15:txfldGUID>
                       <c15:f>calcs!$N$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -4987,7 +4969,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="10"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$O$72</c:f>
@@ -5008,10 +4989,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{E2CE93C5-8A74-40D8-BBDC-8890185EC12F}</c15:txfldGUID>
+                      <c15:txfldGUID>{8FEE8B3C-F158-426C-95CE-376EF5E118A2}</c15:txfldGUID>
                       <c15:f>calcs!$O$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5030,7 +5010,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="11"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$P$72</c:f>
@@ -5051,10 +5030,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{A3C8D572-4DEE-4469-9B11-4A8F56787A17}</c15:txfldGUID>
+                      <c15:txfldGUID>{45178EF0-0FD2-4002-BD90-B1546CA70DA1}</c15:txfldGUID>
                       <c15:f>calcs!$P$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5073,7 +5051,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="12"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$Q$72</c:f>
@@ -5094,10 +5071,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{747E5B4B-05BD-4BBB-9030-FB62465BC77B}</c15:txfldGUID>
+                      <c15:txfldGUID>{7B3CC4CD-9775-4825-A345-44E9ADEB7464}</c15:txfldGUID>
                       <c15:f>calcs!$Q$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5116,7 +5092,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="13"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$R$72</c:f>
@@ -5137,10 +5112,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{71DC3D67-D9C2-4ACF-8DE7-529CFC0D3DC6}</c15:txfldGUID>
+                      <c15:txfldGUID>{BF66E367-7B6D-4EF2-AFEA-07A34BE63824}</c15:txfldGUID>
                       <c15:f>calcs!$R$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5159,7 +5133,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="14"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$S$72</c:f>
@@ -5180,10 +5153,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{624EFDFA-4620-4A8E-8B18-A38E52913C1A}</c15:txfldGUID>
+                      <c15:txfldGUID>{3ED90C93-C56E-4C17-9DC1-174B2B65BD75}</c15:txfldGUID>
                       <c15:f>calcs!$S$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5202,7 +5174,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="15"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$T$72</c:f>
@@ -5223,10 +5194,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{5790453A-FE26-42CA-954C-BB95C5CD40FA}</c15:txfldGUID>
+                      <c15:txfldGUID>{FAAEAF00-E3F5-4E4C-AB48-88B679D3619B}</c15:txfldGUID>
                       <c15:f>calcs!$T$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5245,7 +5215,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="16"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$U$72</c:f>
@@ -5266,10 +5235,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{DD0EEDAB-507E-4952-B311-E4BFD29869A0}</c15:txfldGUID>
+                      <c15:txfldGUID>{5725D353-9DA7-474B-A702-333C49F4204F}</c15:txfldGUID>
                       <c15:f>calcs!$U$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5288,7 +5256,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="17"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$V$72</c:f>
@@ -5309,10 +5276,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{2347195A-6AB4-4F75-9C31-1F056360DB56}</c15:txfldGUID>
+                      <c15:txfldGUID>{19FB9C91-AC05-4D39-9D66-5F338437ED0A}</c15:txfldGUID>
                       <c15:f>calcs!$V$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5331,7 +5297,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="18"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$W$72</c:f>
@@ -5352,10 +5317,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{074DE19A-1044-45D1-A090-28B2B6C89748}</c15:txfldGUID>
+                      <c15:txfldGUID>{C17D96D0-8D7F-4825-AD47-3E7198053CE7}</c15:txfldGUID>
                       <c15:f>calcs!$W$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5374,7 +5338,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="19"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$X$72</c:f>
@@ -5395,10 +5358,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{98621D87-F8C9-42AE-903C-71302EE7EAD3}</c15:txfldGUID>
+                      <c15:txfldGUID>{7E529747-9B3A-4522-9291-D47E782080A1}</c15:txfldGUID>
                       <c15:f>calcs!$X$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5417,7 +5379,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="20"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$Y$72</c:f>
@@ -5438,10 +5399,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{03A0B14B-3DDA-47FB-9E6D-533A0C5D4D53}</c15:txfldGUID>
+                      <c15:txfldGUID>{24995C0F-6C84-43CA-9D57-A530D501472D}</c15:txfldGUID>
                       <c15:f>calcs!$Y$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5460,7 +5420,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="21"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$Z$72</c:f>
@@ -5481,10 +5440,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{60919BA9-EC89-4609-A462-8A848DD27366}</c15:txfldGUID>
+                      <c15:txfldGUID>{58E423F0-90B3-459A-8448-243FC00842FA}</c15:txfldGUID>
                       <c15:f>calcs!$Z$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5503,7 +5461,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="22"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$AA$72</c:f>
@@ -5524,10 +5481,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{CD07B6DC-BACB-4352-BFBD-1128D2CADD81}</c15:txfldGUID>
+                      <c15:txfldGUID>{9787D0E5-0326-439B-B654-3679E41EDFAA}</c15:txfldGUID>
                       <c15:f>calcs!$AA$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5546,7 +5502,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="23"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$AB$72</c:f>
@@ -5567,10 +5522,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{4985242D-EE7C-4E93-982B-F6173111D9D2}</c15:txfldGUID>
+                      <c15:txfldGUID>{CCDAA3CB-9146-437E-B244-B6040B6DFDCF}</c15:txfldGUID>
                       <c15:f>calcs!$AB$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5589,7 +5543,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="24"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$AC$72</c:f>
@@ -5610,10 +5563,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{4E603FF7-5191-4EAB-87A3-4C11EF50C647}</c15:txfldGUID>
+                      <c15:txfldGUID>{AA1D9CEF-A365-4ADC-9D91-EF0C9CEE7442}</c15:txfldGUID>
                       <c15:f>calcs!$AC$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5632,7 +5584,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="25"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$AD$72</c:f>
@@ -5653,10 +5604,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{D05CB611-5C4D-492B-AF17-2AC55572DF42}</c15:txfldGUID>
+                      <c15:txfldGUID>{333C205D-53CC-4BBA-9713-76A4112A5B3F}</c15:txfldGUID>
                       <c15:f>calcs!$AD$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5675,7 +5625,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="26"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$AE$72</c:f>
@@ -5696,10 +5645,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{7269095A-4E07-4E47-A31A-06D9DF59CA56}</c15:txfldGUID>
+                      <c15:txfldGUID>{38C16B32-08BF-435D-B38E-C1863AA2430D}</c15:txfldGUID>
                       <c15:f>calcs!$AE$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5718,7 +5666,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="27"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$AF$72</c:f>
@@ -5739,10 +5686,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{0029A868-BB31-4F02-AC0B-345465BC7B3E}</c15:txfldGUID>
+                      <c15:txfldGUID>{29A2094D-B701-41CB-9720-69C1684DE401}</c15:txfldGUID>
                       <c15:f>calcs!$AF$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5761,7 +5707,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="28"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$AG$72</c:f>
@@ -5782,10 +5727,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{CE71FF7D-F630-4A11-B1D1-4095A9BF08FF}</c15:txfldGUID>
+                      <c15:txfldGUID>{524EDC19-231D-42EE-B120-B1FC51CE47AA}</c15:txfldGUID>
                       <c15:f>calcs!$AG$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5804,7 +5748,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="29"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$AH$72</c:f>
@@ -5825,10 +5768,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{5FB4D70A-CD28-4C9C-ACAE-978F3C5FE460}</c15:txfldGUID>
+                      <c15:txfldGUID>{D2480BE9-49AA-4FFD-9CD8-27757D7B8FCD}</c15:txfldGUID>
                       <c15:f>calcs!$AH$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5999,7 +5941,6 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$E$70</c:f>
@@ -6020,10 +5961,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{C108E296-EB9D-4981-B429-AF70D74D78A2}</c15:txfldGUID>
+                      <c15:txfldGUID>{7B60E4CC-C746-4A6D-9D4A-297B965E2FA7}</c15:txfldGUID>
                       <c15:f>calcs!$E$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6042,7 +5982,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$F$70</c:f>
@@ -6063,10 +6002,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{6F958A22-9139-4CD8-93C8-4A0E03F985E5}</c15:txfldGUID>
+                      <c15:txfldGUID>{0ED9359A-55A7-4A3C-9341-4655D3BA3127}</c15:txfldGUID>
                       <c15:f>calcs!$F$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6085,7 +6023,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$G$70</c:f>
@@ -6106,10 +6043,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{AF17D408-35EA-42C9-A210-CE54072D13C3}</c15:txfldGUID>
+                      <c15:txfldGUID>{99B86E59-2A2F-4DF1-8D5E-329E4CE29A16}</c15:txfldGUID>
                       <c15:f>calcs!$G$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6128,7 +6064,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$H$70</c:f>
@@ -6149,10 +6084,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{3F6F63C9-242D-4A0A-A229-D106C8DBC1C1}</c15:txfldGUID>
+                      <c15:txfldGUID>{2810ADD8-688B-4A60-BD24-38780BB930D7}</c15:txfldGUID>
                       <c15:f>calcs!$H$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6171,7 +6105,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$I$70</c:f>
@@ -6192,10 +6125,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{44BEFF4A-F6D0-438D-91F3-C38BEADE57E9}</c15:txfldGUID>
+                      <c15:txfldGUID>{0410F87A-99D0-462A-AE5A-E3B7CE014A64}</c15:txfldGUID>
                       <c15:f>calcs!$I$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6214,7 +6146,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="5"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$J$70</c:f>
@@ -6235,10 +6166,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{D9B57202-C9BD-4D01-AF25-579EAD35A8B6}</c15:txfldGUID>
+                      <c15:txfldGUID>{0D981FFC-3823-4C5F-ACF1-AB9BFFC148B3}</c15:txfldGUID>
                       <c15:f>calcs!$J$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6257,7 +6187,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="6"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$K$70</c:f>
@@ -6278,10 +6207,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{2E19D1AC-14F4-4C5B-B291-F06D9D353416}</c15:txfldGUID>
+                      <c15:txfldGUID>{3A832B65-8FEB-47F7-A393-B185F1821207}</c15:txfldGUID>
                       <c15:f>calcs!$K$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6300,7 +6228,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="7"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$L$70</c:f>
@@ -6321,10 +6248,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{76260412-B1C0-4FA6-8A0D-B1718406EE7A}</c15:txfldGUID>
+                      <c15:txfldGUID>{3127E490-E631-4AAF-A32F-88D9171B7E58}</c15:txfldGUID>
                       <c15:f>calcs!$L$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6343,7 +6269,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="8"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$M$70</c:f>
@@ -6364,10 +6289,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{6D71727B-5691-4A33-AD7A-23DA98FA9F92}</c15:txfldGUID>
+                      <c15:txfldGUID>{561FF2D3-384F-4FA7-BE1B-D064C6D78290}</c15:txfldGUID>
                       <c15:f>calcs!$M$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6386,7 +6310,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="9"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$N$70</c:f>
@@ -6407,10 +6330,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{41A0D359-C874-48A6-B73B-90F1457E1DA6}</c15:txfldGUID>
+                      <c15:txfldGUID>{C6E1C7A4-543F-41A6-8AF1-995D62FF7FBA}</c15:txfldGUID>
                       <c15:f>calcs!$N$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6429,7 +6351,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="10"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$O$70</c:f>
@@ -6450,10 +6371,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{D0D1C6FA-4DDC-4D53-8575-40019A29BD06}</c15:txfldGUID>
+                      <c15:txfldGUID>{8AA96064-1BFD-4CFE-A623-B59FC3D149C2}</c15:txfldGUID>
                       <c15:f>calcs!$O$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6472,7 +6392,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="11"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$P$70</c:f>
@@ -6493,10 +6412,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{10C0C692-00A9-466C-AD3D-EB8C85A9BA83}</c15:txfldGUID>
+                      <c15:txfldGUID>{DE043912-DF88-45C5-8EC7-F3CCFDF018D5}</c15:txfldGUID>
                       <c15:f>calcs!$P$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6515,7 +6433,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="12"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$Q$70</c:f>
@@ -6536,10 +6453,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{12962FA9-BB66-4A63-BA90-6F6083AF70B3}</c15:txfldGUID>
+                      <c15:txfldGUID>{85202FFA-DF19-4C9E-B63C-2DB604C2B7D7}</c15:txfldGUID>
                       <c15:f>calcs!$Q$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6558,7 +6474,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="13"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$R$70</c:f>
@@ -6579,10 +6494,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{FD27C8DC-5375-4D9B-9792-0F92410C2BFA}</c15:txfldGUID>
+                      <c15:txfldGUID>{28AB5647-6935-40DC-9B63-D991997DCCA0}</c15:txfldGUID>
                       <c15:f>calcs!$R$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6601,7 +6515,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="14"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$S$70</c:f>
@@ -6622,10 +6535,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{4179F873-CAC1-4C09-A065-7D4AB6E00521}</c15:txfldGUID>
+                      <c15:txfldGUID>{C4471918-50F8-4293-8183-42C13D9D9667}</c15:txfldGUID>
                       <c15:f>calcs!$S$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6644,7 +6556,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="15"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$T$70</c:f>
@@ -6665,10 +6576,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{8B614FA4-9CE4-42FB-82C5-FE791C8D598D}</c15:txfldGUID>
+                      <c15:txfldGUID>{D1868024-139C-4CC1-B6CB-4F07A1B6FC89}</c15:txfldGUID>
                       <c15:f>calcs!$T$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6687,7 +6597,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="16"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$U$70</c:f>
@@ -6708,10 +6617,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{29102A39-D507-4156-B4DD-B81B4F52C230}</c15:txfldGUID>
+                      <c15:txfldGUID>{C7190F37-4102-48E4-8338-FF35A779FDAC}</c15:txfldGUID>
                       <c15:f>calcs!$U$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6730,7 +6638,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="17"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$V$70</c:f>
@@ -6751,10 +6658,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{BB2A1235-CD19-4BD3-8116-6B53F5989F87}</c15:txfldGUID>
+                      <c15:txfldGUID>{A9D62DD2-974B-4E9D-BC20-54F120F8EB87}</c15:txfldGUID>
                       <c15:f>calcs!$V$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6773,7 +6679,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="18"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$W$70</c:f>
@@ -6794,10 +6699,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{11829C7F-9ACC-463B-88E2-3F0C9924131A}</c15:txfldGUID>
+                      <c15:txfldGUID>{19D0682C-FF2E-4900-A8FF-1BFF73EE9860}</c15:txfldGUID>
                       <c15:f>calcs!$W$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6816,7 +6720,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="19"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$X$70</c:f>
@@ -6837,10 +6740,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{516CE411-3BC9-4FA4-A9B4-1CE3C671A61A}</c15:txfldGUID>
+                      <c15:txfldGUID>{4EAD5E23-77D0-4369-9A71-ABAB48F790D9}</c15:txfldGUID>
                       <c15:f>calcs!$X$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6859,7 +6761,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="20"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$Y$70</c:f>
@@ -6880,10 +6781,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{0F4BF786-0CC3-419B-B77D-4E80286B0A5F}</c15:txfldGUID>
+                      <c15:txfldGUID>{03FEC568-7506-4B08-BE58-D01D98608A9B}</c15:txfldGUID>
                       <c15:f>calcs!$Y$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6902,7 +6802,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="21"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$Z$70</c:f>
@@ -6923,10 +6822,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{74FC716F-FA30-4CB9-B041-2C0B88B1E7A5}</c15:txfldGUID>
+                      <c15:txfldGUID>{70E31AFA-B687-46AC-909B-34AF2971FF8D}</c15:txfldGUID>
                       <c15:f>calcs!$Z$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6945,7 +6843,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="22"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$AA$70</c:f>
@@ -6966,10 +6863,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{D77E471A-2137-48C9-AA9F-40A356CBC6A8}</c15:txfldGUID>
+                      <c15:txfldGUID>{751847D7-2DE3-4A5F-A483-D672BA3ED997}</c15:txfldGUID>
                       <c15:f>calcs!$AA$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6988,7 +6884,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="23"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$AB$70</c:f>
@@ -7009,10 +6904,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{7874B4E0-388C-497E-B0B6-474003AE562B}</c15:txfldGUID>
+                      <c15:txfldGUID>{179F0E95-ADFF-4D4B-8C6B-3E57826B440C}</c15:txfldGUID>
                       <c15:f>calcs!$AB$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -7031,7 +6925,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="24"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$AC$70</c:f>
@@ -7052,10 +6945,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{CB02BCEB-3B49-436A-B88B-40052413874A}</c15:txfldGUID>
+                      <c15:txfldGUID>{BD47ED62-A736-49D0-8E63-BF8BD0AE920E}</c15:txfldGUID>
                       <c15:f>calcs!$AC$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -7074,7 +6966,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="25"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$AD$70</c:f>
@@ -7095,10 +6986,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{F36C4176-83CB-4540-B5B6-D58A863FF5EB}</c15:txfldGUID>
+                      <c15:txfldGUID>{B55C891E-F31B-4ECD-AF75-7A42C67221F9}</c15:txfldGUID>
                       <c15:f>calcs!$AD$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -7117,7 +7007,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="26"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$AE$70</c:f>
@@ -7138,10 +7027,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{1AFC544F-812A-4EC9-9385-973144551E14}</c15:txfldGUID>
+                      <c15:txfldGUID>{448FBA0F-B234-4103-9128-DB59A3FD0522}</c15:txfldGUID>
                       <c15:f>calcs!$AE$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -7160,7 +7048,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="27"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$AF$70</c:f>
@@ -7181,10 +7068,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{7184A0A4-9460-4B6F-B295-963473812CE7}</c15:txfldGUID>
+                      <c15:txfldGUID>{28FBB445-9C3C-4B4A-9D27-671D11E1F944}</c15:txfldGUID>
                       <c15:f>calcs!$AF$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -7203,7 +7089,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="28"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$AG$70</c:f>
@@ -7224,10 +7109,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{331FC590-DBBD-4CB0-A9AB-50297B51E010}</c15:txfldGUID>
+                      <c15:txfldGUID>{C123DB92-9171-4378-8397-086D6A7BA561}</c15:txfldGUID>
                       <c15:f>calcs!$AG$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -7246,7 +7130,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="29"/>
-              <c:layout/>
               <c:tx>
                 <c:strRef>
                   <c:f>calcs!$AH$70</c:f>
@@ -7267,10 +7150,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{C633C9ED-B1BF-456F-9DD8-EA859A98CDCD}</c15:txfldGUID>
+                      <c15:txfldGUID>{3EA59EAB-C804-437E-A830-FE75B7AEC473}</c15:txfldGUID>
                       <c15:f>calcs!$AH$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -7849,8 +7731,8 @@
         <a:xfrm>
           <a:off x="325877" y="4038600"/>
           <a:ext cx="8988869" cy="228436"/>
-          <a:chOff x="306828" y="4108026"/>
-          <a:chExt cx="8729080" cy="223568"/>
+          <a:chOff x="306828" y="4108028"/>
+          <a:chExt cx="8729080" cy="223566"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
@@ -7924,7 +7806,7 @@
             </xdr:nvSpPr>
             <xdr:spPr bwMode="auto">
               <a:xfrm>
-                <a:off x="306828" y="4108026"/>
+                <a:off x="306828" y="4108028"/>
                 <a:ext cx="8729080" cy="163196"/>
               </a:xfrm>
               <a:prstGeom prst="rect">
@@ -7948,23 +7830,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Activities" displayName="Activities" ref="B4:F16" totalsRowShown="0">
-  <autoFilter ref="B4:F16"/>
-  <sortState ref="C19:F24">
-    <sortCondition ref="D18:D24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Activities" displayName="Activities" ref="B4:F17" totalsRowShown="0">
+  <autoFilter ref="B4:F17" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C20:F25">
+    <sortCondition ref="D19:D25"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="5" name="Id">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Id">
       <calculatedColumnFormula>ROW(B5)-calcs!$D$5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="ACTIVITY" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="START">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ACTIVITY" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="START">
       <calculatedColumnFormula>D4+10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="END">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="END">
       <calculatedColumnFormula>Activities[[#This Row],[START]]+2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="NOTES"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="NOTES"/>
   </tableColumns>
   <tableStyleInfo name="Project Timeline" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -8201,15 +8083,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1">
     <tabColor theme="6" tint="-0.249977111117893"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8271,7 +8153,7 @@
     <row r="5" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5">
         <f>ROW(B5)-calcs!$D$5</f>
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="C5" t="s">
         <v>22</v>
@@ -8290,7 +8172,7 @@
     <row r="6" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6">
         <f>ROW(B6)-calcs!$D$5</f>
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="C6" t="s">
         <v>23</v>
@@ -8306,7 +8188,7 @@
     <row r="7" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7">
         <f>ROW(B7)-calcs!$D$5</f>
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="C7" t="s">
         <v>24</v>
@@ -8322,7 +8204,7 @@
     <row r="8" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8">
         <f>ROW(B8)-calcs!$D$5</f>
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="C8" t="s">
         <v>25</v>
@@ -8341,7 +8223,7 @@
     <row r="9" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9">
         <f>ROW(B9)-calcs!$D$5</f>
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="C9" t="s">
         <v>29</v>
@@ -8358,7 +8240,7 @@
     <row r="10" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10">
         <f>ROW(B10)-calcs!$D$5</f>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="C10" t="s">
         <v>28</v>
@@ -8378,7 +8260,7 @@
     <row r="11" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11">
         <f>ROW(B11)-calcs!$D$5</f>
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="C11" t="s">
         <v>31</v>
@@ -8395,7 +8277,7 @@
     <row r="12" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12">
         <f>ROW(B12)-calcs!$D$5</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="C12" t="s">
         <v>32</v>
@@ -8415,13 +8297,13 @@
     <row r="13" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13">
         <f>ROW(B13)-calcs!$D$5</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" t="s">
         <v>36</v>
       </c>
       <c r="D13" s="5">
-        <f t="shared" ref="D10:D15" si="0">D12+7</f>
+        <f t="shared" ref="D13" si="0">D12+7</f>
         <v>43788</v>
       </c>
       <c r="E13" s="5">
@@ -8435,7 +8317,7 @@
     <row r="14" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14">
         <f>ROW(B14)-calcs!$D$5</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14" t="s">
         <v>34</v>
@@ -8455,7 +8337,7 @@
     <row r="15" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15">
         <f>ROW(B15)-calcs!$D$5</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C15" t="s">
         <v>38</v>
@@ -8475,15 +8357,34 @@
     <row r="16" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16">
         <f>ROW(B16)-calcs!$D$5</f>
+        <v>3</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="5">
+        <v>43801</v>
+      </c>
+      <c r="E16" s="5">
+        <f>Activities[[#This Row],[START]]+2</f>
+        <v>43803</v>
+      </c>
+      <c r="F16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <f>ROW(B17)-calcs!$D$5</f>
         <v>4</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D17" s="5">
         <v>43806</v>
       </c>
-      <c r="E16" s="5"/>
+      <c r="E17" s="5"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
@@ -8492,14 +8393,14 @@
     <mergeCell ref="C2:G2"/>
   </mergeCells>
   <dataValidations count="8">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Create a Project Timeline in this worksheet. Enter project Start Date in cell D3 and project details in Activities table. Timeline charting project activities is in cell C2" sqref="A1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of this worksheet is in this cell. Timeline chart depicting scrollable timeline of the project activities is in cell below" sqref="C1:G1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Start Date in cell at right" sqref="C3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Start Date in this cell and project details in table below" sqref="D3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter project Activity in this column under this heading. Use heading filters to find specific entries" sqref="C4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Start date in this column under this heading" sqref="D4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter End date in this column under this heading" sqref="E4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Notes in this column under this heading" sqref="F4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Create a Project Timeline in this worksheet. Enter project Start Date in cell D3 and project details in Activities table. Timeline charting project activities is in cell C2" sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of this worksheet is in this cell. Timeline chart depicting scrollable timeline of the project activities is in cell below" sqref="C1:G1" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Start Date in cell at right" sqref="C3" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Start Date in this cell and project details in table below" sqref="D3" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter project Activity in this column under this heading. Use heading filters to find specific entries" sqref="C4" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Start date in this column under this heading" sqref="D4" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter End date in this column under this heading" sqref="E4" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Notes in this column under this heading" sqref="F4" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
@@ -8544,7 +8445,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AI72"/>
   <sheetViews>
@@ -8571,7 +8472,7 @@
       </c>
       <c r="D3" s="1">
         <f ca="1">TODAY()</f>
-        <v>43790</v>
+        <v>43802</v>
       </c>
       <c r="E3" s="1"/>
     </row>
@@ -8586,7 +8487,7 @@
       </c>
       <c r="D5">
         <f>ROWS(Activities[])</f>
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -8663,7 +8564,7 @@
       <c r="C15" s="2"/>
       <c r="E15">
         <f t="array" ref="E15">INDEX(Activities[Id],MATCH(1, ((Activities[START]&gt;=StartDateWindow)+(Activities[END]&gt;=StartDateWindow)&gt;0)*(Activities[START]&lt;=(StartDateWindow+WindowDays-1)), 0))</f>
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="F15" t="e">
         <f t="shared" ref="F15:F23" ca="1" si="0">OFFSET(E15,-$D$11,)</f>
@@ -8674,7 +8575,7 @@
       <c r="C16" s="2"/>
       <c r="E16">
         <f t="array" ref="E16">INDEX(Activities[Id],MATCH(1, (Activities[Id]&gt;E15)*((Activities[START]&gt;=StartDateWindow)+(Activities[END]&gt;=StartDateWindow)&gt;0)*(Activities[START]&lt;=(StartDateWindow+WindowDays-1)), 0))</f>
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="F16" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -8685,7 +8586,7 @@
       <c r="C17" s="2"/>
       <c r="E17">
         <f t="array" ref="E17">INDEX(Activities[Id],MATCH(1, (Activities[Id]&gt;E16)*((Activities[START]&gt;=StartDateWindow)+(Activities[END]&gt;=StartDateWindow)&gt;0)*(Activities[START]&lt;=(StartDateWindow+WindowDays-1)), 0))</f>
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="F17" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -8729,7 +8630,7 @@
       </c>
       <c r="F21">
         <f t="shared" ca="1" si="0"/>
-        <v>-7</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.25">
@@ -8739,7 +8640,7 @@
       </c>
       <c r="F22">
         <f t="shared" ca="1" si="0"/>
-        <v>-6</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.25">
@@ -8749,7 +8650,7 @@
       </c>
       <c r="F23">
         <f t="shared" ca="1" si="0"/>
-        <v>-5</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="25" spans="1:35" ht="30" x14ac:dyDescent="0.25">
@@ -9769,7 +9670,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:35" ht="30" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="3"/>
         <v>5.3000000000000007</v>
@@ -9779,7 +9680,7 @@
       </c>
       <c r="C38">
         <f t="shared" ca="1" si="2"/>
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="D38" t="str">
         <f ca="1">INDEX(Activities[ACTIVITY],MATCH($C38,Activities[Id],0))</f>
@@ -9910,7 +9811,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:35" ht="30" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="3"/>
         <v>4.3000000000000007</v>
@@ -9920,7 +9821,7 @@
       </c>
       <c r="C39">
         <f t="shared" ca="1" si="2"/>
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="D39" t="str">
         <f ca="1">INDEX(Activities[ACTIVITY],MATCH($C39,Activities[Id],0))</f>
@@ -10051,7 +9952,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:35" ht="30" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="3"/>
         <v>3.3000000000000007</v>
@@ -10061,7 +9962,7 @@
       </c>
       <c r="C40">
         <f t="shared" ca="1" si="2"/>
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="D40" t="str">
         <f ca="1">INDEX(Activities[ACTIVITY],MATCH($C40,Activities[Id],0))</f>
@@ -11094,10 +10995,10 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="50" spans="3:34" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:34" ht="30" x14ac:dyDescent="0.25">
       <c r="C50">
         <f t="shared" ca="1" si="6"/>
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="D50" t="str">
         <f ca="1">UPPER(INDEX(Activities[ACTIVITY],MATCH($C50,Activities[Id],0)))</f>
@@ -11224,10 +11125,10 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="51" spans="3:34" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:34" ht="45" x14ac:dyDescent="0.25">
       <c r="C51">
         <f t="shared" ca="1" si="6"/>
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="D51" t="str">
         <f ca="1">UPPER(INDEX(Activities[ACTIVITY],MATCH($C51,Activities[Id],0)))</f>
@@ -11354,10 +11255,10 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="52" spans="3:34" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:34" ht="30" x14ac:dyDescent="0.25">
       <c r="C52">
         <f t="shared" ca="1" si="6"/>
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="D52" t="str">
         <f ca="1">UPPER(INDEX(Activities[ACTIVITY],MATCH($C52,Activities[Id],0)))</f>
@@ -12989,6 +12890,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9677210f24a1be23c92c90fd886aa0aa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="60e05723c5c1908df1a1a4ebf11d344e" ns2:_="" ns3:_="">
     <xsd:import namespace="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
@@ -13199,24 +13117,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{983CAFE3-5C64-4732-BD1D-A9D00643597D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED11D93F-21D3-4821-9768-A0F99C41A8EB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5BB6EA-B4A9-4FD0-A581-32FE787E0D00}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13233,22 +13152,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED11D93F-21D3-4821-9768-A0F99C41A8EB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{983CAFE3-5C64-4732-BD1D-A9D00643597D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
moved folders of project for rename
</commit_message>
<xml_diff>
--- a/Documentation/project timeline.xlsx
+++ b/Documentation/project timeline.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C47973E-2C92-49EE-A090-D8F86F5AA9E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA7B918A-A0C1-4E3C-B0D1-CFE4A063BDC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Activity</t>
   </si>
@@ -161,6 +161,9 @@
   </si>
   <si>
     <t>Abandonment</t>
+  </si>
+  <si>
+    <t>Final Presentation</t>
   </si>
 </sst>
 </file>
@@ -388,14 +391,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
@@ -556,94 +559,94 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>43713</c:v>
+                  <c:v>43720</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43714</c:v>
+                  <c:v>43721</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43715</c:v>
+                  <c:v>43722</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43716</c:v>
+                  <c:v>43723</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43717</c:v>
+                  <c:v>43724</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43718</c:v>
+                  <c:v>43725</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43719</c:v>
+                  <c:v>43726</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43720</c:v>
+                  <c:v>43727</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43721</c:v>
+                  <c:v>43728</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43722</c:v>
+                  <c:v>43729</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43723</c:v>
+                  <c:v>43730</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43724</c:v>
+                  <c:v>43731</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43725</c:v>
+                  <c:v>43732</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43726</c:v>
+                  <c:v>43733</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43727</c:v>
+                  <c:v>43734</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43728</c:v>
+                  <c:v>43735</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43729</c:v>
+                  <c:v>43736</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>43730</c:v>
+                  <c:v>43737</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>43731</c:v>
+                  <c:v>43738</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>43732</c:v>
+                  <c:v>43739</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>43733</c:v>
+                  <c:v>43740</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>43734</c:v>
+                  <c:v>43741</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>43735</c:v>
+                  <c:v>43742</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>43736</c:v>
+                  <c:v>43743</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>43737</c:v>
+                  <c:v>43744</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>43738</c:v>
+                  <c:v>43745</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>43739</c:v>
+                  <c:v>43746</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>43740</c:v>
+                  <c:v>43747</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>43741</c:v>
+                  <c:v>43748</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>43742</c:v>
+                  <c:v>43749</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -950,94 +953,94 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>43713</c:v>
+                  <c:v>43720</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43714</c:v>
+                  <c:v>43721</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43715</c:v>
+                  <c:v>43722</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43716</c:v>
+                  <c:v>43723</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43717</c:v>
+                  <c:v>43724</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43718</c:v>
+                  <c:v>43725</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43719</c:v>
+                  <c:v>43726</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43720</c:v>
+                  <c:v>43727</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43721</c:v>
+                  <c:v>43728</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43722</c:v>
+                  <c:v>43729</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43723</c:v>
+                  <c:v>43730</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43724</c:v>
+                  <c:v>43731</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43725</c:v>
+                  <c:v>43732</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43726</c:v>
+                  <c:v>43733</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43727</c:v>
+                  <c:v>43734</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43728</c:v>
+                  <c:v>43735</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43729</c:v>
+                  <c:v>43736</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>43730</c:v>
+                  <c:v>43737</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>43731</c:v>
+                  <c:v>43738</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>43732</c:v>
+                  <c:v>43739</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>43733</c:v>
+                  <c:v>43740</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>43734</c:v>
+                  <c:v>43741</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>43735</c:v>
+                  <c:v>43742</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>43736</c:v>
+                  <c:v>43743</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>43737</c:v>
+                  <c:v>43744</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>43738</c:v>
+                  <c:v>43745</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>43739</c:v>
+                  <c:v>43746</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>43740</c:v>
+                  <c:v>43747</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>43741</c:v>
+                  <c:v>43748</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>43742</c:v>
+                  <c:v>43749</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1344,94 +1347,94 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>43713</c:v>
+                  <c:v>43720</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43714</c:v>
+                  <c:v>43721</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43715</c:v>
+                  <c:v>43722</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43716</c:v>
+                  <c:v>43723</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43717</c:v>
+                  <c:v>43724</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43718</c:v>
+                  <c:v>43725</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43719</c:v>
+                  <c:v>43726</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43720</c:v>
+                  <c:v>43727</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43721</c:v>
+                  <c:v>43728</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43722</c:v>
+                  <c:v>43729</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43723</c:v>
+                  <c:v>43730</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43724</c:v>
+                  <c:v>43731</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43725</c:v>
+                  <c:v>43732</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43726</c:v>
+                  <c:v>43733</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43727</c:v>
+                  <c:v>43734</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43728</c:v>
+                  <c:v>43735</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43729</c:v>
+                  <c:v>43736</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>43730</c:v>
+                  <c:v>43737</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>43731</c:v>
+                  <c:v>43738</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>43732</c:v>
+                  <c:v>43739</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>43733</c:v>
+                  <c:v>43740</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>43734</c:v>
+                  <c:v>43741</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>43735</c:v>
+                  <c:v>43742</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>43736</c:v>
+                  <c:v>43743</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>43737</c:v>
+                  <c:v>43744</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>43738</c:v>
+                  <c:v>43745</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>43739</c:v>
+                  <c:v>43746</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>43740</c:v>
+                  <c:v>43747</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>43741</c:v>
+                  <c:v>43748</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>43742</c:v>
+                  <c:v>43749</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1747,94 +1750,94 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>43713</c:v>
+                  <c:v>43720</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43714</c:v>
+                  <c:v>43721</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43715</c:v>
+                  <c:v>43722</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43716</c:v>
+                  <c:v>43723</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43717</c:v>
+                  <c:v>43724</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43718</c:v>
+                  <c:v>43725</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43719</c:v>
+                  <c:v>43726</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43720</c:v>
+                  <c:v>43727</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43721</c:v>
+                  <c:v>43728</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43722</c:v>
+                  <c:v>43729</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43723</c:v>
+                  <c:v>43730</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43724</c:v>
+                  <c:v>43731</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43725</c:v>
+                  <c:v>43732</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43726</c:v>
+                  <c:v>43733</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43727</c:v>
+                  <c:v>43734</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43728</c:v>
+                  <c:v>43735</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43729</c:v>
+                  <c:v>43736</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>43730</c:v>
+                  <c:v>43737</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>43731</c:v>
+                  <c:v>43738</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>43732</c:v>
+                  <c:v>43739</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>43733</c:v>
+                  <c:v>43740</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>43734</c:v>
+                  <c:v>43741</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>43735</c:v>
+                  <c:v>43742</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>43736</c:v>
+                  <c:v>43743</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>43737</c:v>
+                  <c:v>43744</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>43738</c:v>
+                  <c:v>43745</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>43739</c:v>
+                  <c:v>43746</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>43740</c:v>
+                  <c:v>43747</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>43741</c:v>
+                  <c:v>43748</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>43742</c:v>
+                  <c:v>43749</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2141,94 +2144,94 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>43713</c:v>
+                  <c:v>43720</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43714</c:v>
+                  <c:v>43721</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43715</c:v>
+                  <c:v>43722</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43716</c:v>
+                  <c:v>43723</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43717</c:v>
+                  <c:v>43724</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43718</c:v>
+                  <c:v>43725</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43719</c:v>
+                  <c:v>43726</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43720</c:v>
+                  <c:v>43727</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43721</c:v>
+                  <c:v>43728</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43722</c:v>
+                  <c:v>43729</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43723</c:v>
+                  <c:v>43730</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43724</c:v>
+                  <c:v>43731</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43725</c:v>
+                  <c:v>43732</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43726</c:v>
+                  <c:v>43733</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43727</c:v>
+                  <c:v>43734</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43728</c:v>
+                  <c:v>43735</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43729</c:v>
+                  <c:v>43736</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>43730</c:v>
+                  <c:v>43737</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>43731</c:v>
+                  <c:v>43738</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>43732</c:v>
+                  <c:v>43739</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>43733</c:v>
+                  <c:v>43740</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>43734</c:v>
+                  <c:v>43741</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>43735</c:v>
+                  <c:v>43742</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>43736</c:v>
+                  <c:v>43743</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>43737</c:v>
+                  <c:v>43744</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>43738</c:v>
+                  <c:v>43745</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>43739</c:v>
+                  <c:v>43746</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>43740</c:v>
+                  <c:v>43747</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>43741</c:v>
+                  <c:v>43748</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>43742</c:v>
+                  <c:v>43749</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2877,58 +2880,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>5.3000000000000007</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="11">
                   <c:v>5.3000000000000007</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="12">
                   <c:v>5.3000000000000007</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="13">
                   <c:v>5.3000000000000007</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>#N/A</c:v>
-                </c:pt>
                 <c:pt idx="14">
-                  <c:v>#N/A</c:v>
+                  <c:v>5.3000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>#N/A</c:v>
+                  <c:v>5.3000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>#N/A</c:v>
+                  <c:v>5.3000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>#N/A</c:v>
+                  <c:v>5.3000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>#N/A</c:v>
@@ -2985,7 +2988,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>PARTNERING &amp; BRAINSTORMING</c:v>
+                  <c:v>LATEX DOCUMENTATION 1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3059,49 +3062,49 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>5.3000000000000007</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>#N/A</c:v>
@@ -3260,10 +3263,10 @@
                   <c:v>4.3000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>#N/A</c:v>
+                  <c:v>4.3000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>#N/A</c:v>
+                  <c:v>4.3000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>#N/A</c:v>
@@ -3293,7 +3296,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>LATEX DOCUMENTATION 1</c:v>
+                  <c:v>PROJECT SCOPE ESTABLISHED</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3430,13 +3433,13 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="24">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>4.3000000000000007</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>#N/A</c:v>
@@ -3565,10 +3568,10 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3.3000000000000007</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3.3000000000000007</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>3.3000000000000007</c:v>
@@ -3601,7 +3604,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>PROJECT SCOPE ESTABLISHED</c:v>
+                  <c:v>LATEX DOCUMENTATION 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3987,25 +3990,25 @@
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.5</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.5</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.5</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.5</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.5</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.5</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.5</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>#N/A</c:v>
@@ -4120,25 +4123,25 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>#N/A</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>#N/A</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>#N/A</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>#N/A</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>#N/A</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>#N/A</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>#N/A</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>0.5</c:v>
@@ -4282,7 +4285,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>#N/A</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>#N/A</c:v>
@@ -4303,7 +4306,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.5</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>#N/A</c:v>
@@ -4565,7 +4568,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>05</c:v>
+                      <c:v>12</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -4581,12 +4584,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{65F84D80-D0F7-48EA-9FEE-93DC87D057CE}</c15:txfldGUID>
+                      <c15:txfldGUID>{60DBB9D3-2CED-4E75-AA09-92EA0D6A6FF5}</c15:txfldGUID>
                       <c15:f>calcs!$E$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>05</c:v>
+                          <c:v>12</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -4606,7 +4609,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>06</c:v>
+                      <c:v>13</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -4622,12 +4625,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{A1540CEE-BA27-42C4-916F-5D5AEE343ADE}</c15:txfldGUID>
+                      <c15:txfldGUID>{8D46CC3C-901A-4BDA-B0FF-4231C5E4F052}</c15:txfldGUID>
                       <c15:f>calcs!$F$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>06</c:v>
+                          <c:v>13</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -4647,7 +4650,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>07</c:v>
+                      <c:v>14</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -4663,12 +4666,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{CF20AFE9-FF4B-4A99-9981-11021F5CA6F9}</c15:txfldGUID>
+                      <c15:txfldGUID>{C30E4C86-920C-4DBD-9A97-8997FBE5E534}</c15:txfldGUID>
                       <c15:f>calcs!$G$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>07</c:v>
+                          <c:v>14</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -4688,7 +4691,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>08</c:v>
+                      <c:v>15</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -4704,12 +4707,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{7EC3A0A0-82A9-4474-9D2C-5133620CB130}</c15:txfldGUID>
+                      <c15:txfldGUID>{A7D1F478-252C-4936-8A9E-FBF4C5467EB7}</c15:txfldGUID>
                       <c15:f>calcs!$H$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>08</c:v>
+                          <c:v>15</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -4729,7 +4732,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>09</c:v>
+                      <c:v>16</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -4745,12 +4748,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{4ED5A793-C57E-4365-AAF6-D05473AA3E77}</c15:txfldGUID>
+                      <c15:txfldGUID>{6CD1C2B1-C211-47E6-A264-C3616D65B98A}</c15:txfldGUID>
                       <c15:f>calcs!$I$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>09</c:v>
+                          <c:v>16</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -4770,7 +4773,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>10</c:v>
+                      <c:v>17</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -4786,12 +4789,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{184C505B-0653-45A6-BEF4-982C8798BC44}</c15:txfldGUID>
+                      <c15:txfldGUID>{9810E9D5-DE0A-457E-BADA-747B6A32C8EA}</c15:txfldGUID>
                       <c15:f>calcs!$J$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>10</c:v>
+                          <c:v>17</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -4811,7 +4814,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>11</c:v>
+                      <c:v>18</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -4827,12 +4830,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{74E52553-E485-49D4-A165-3BF82EB49CAF}</c15:txfldGUID>
+                      <c15:txfldGUID>{F851E054-F46A-4B7E-8B1E-64CAA9D02A41}</c15:txfldGUID>
                       <c15:f>calcs!$K$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>11</c:v>
+                          <c:v>18</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -4852,7 +4855,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>12</c:v>
+                      <c:v>19</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -4868,12 +4871,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{99EC5A5A-C2EF-4C4D-BF12-3575841B5AF3}</c15:txfldGUID>
+                      <c15:txfldGUID>{1556D7BA-0068-4068-A230-33834D0D6969}</c15:txfldGUID>
                       <c15:f>calcs!$L$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>12</c:v>
+                          <c:v>19</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -4893,7 +4896,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>13</c:v>
+                      <c:v>20</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -4909,12 +4912,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{19002E92-295F-4AEF-8A31-BD9A3AC9A6AE}</c15:txfldGUID>
+                      <c15:txfldGUID>{8A39CBE1-DF6F-4D23-AD37-3522DDF2ED61}</c15:txfldGUID>
                       <c15:f>calcs!$M$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>13</c:v>
+                          <c:v>20</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -4934,7 +4937,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>14</c:v>
+                      <c:v>21</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -4950,12 +4953,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{2FA7078C-1B11-490E-8828-DFBF3AF582E4}</c15:txfldGUID>
+                      <c15:txfldGUID>{2E1F0F33-4BBD-4FDD-8663-65625E3FAB1B}</c15:txfldGUID>
                       <c15:f>calcs!$N$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>14</c:v>
+                          <c:v>21</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -4975,7 +4978,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>15</c:v>
+                      <c:v>22</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -4991,12 +4994,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{8FEE8B3C-F158-426C-95CE-376EF5E118A2}</c15:txfldGUID>
+                      <c15:txfldGUID>{B9381A39-B933-4FA7-B3B1-3FFCA6934FB4}</c15:txfldGUID>
                       <c15:f>calcs!$O$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>15</c:v>
+                          <c:v>22</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5016,7 +5019,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>16</c:v>
+                      <c:v>23</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5032,12 +5035,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{45178EF0-0FD2-4002-BD90-B1546CA70DA1}</c15:txfldGUID>
+                      <c15:txfldGUID>{C5C4E512-DA45-4F67-AAB8-E2CC74373BC7}</c15:txfldGUID>
                       <c15:f>calcs!$P$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>16</c:v>
+                          <c:v>23</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5057,7 +5060,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>17</c:v>
+                      <c:v>24</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5073,12 +5076,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{7B3CC4CD-9775-4825-A345-44E9ADEB7464}</c15:txfldGUID>
+                      <c15:txfldGUID>{A7717D06-5DD7-4F46-8A33-E75665C2829F}</c15:txfldGUID>
                       <c15:f>calcs!$Q$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>17</c:v>
+                          <c:v>24</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5098,7 +5101,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>18</c:v>
+                      <c:v>25</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5114,12 +5117,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{BF66E367-7B6D-4EF2-AFEA-07A34BE63824}</c15:txfldGUID>
+                      <c15:txfldGUID>{2DCB816A-4D0B-4F42-B6A5-E17512F3BA44}</c15:txfldGUID>
                       <c15:f>calcs!$R$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>18</c:v>
+                          <c:v>25</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5139,7 +5142,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>19</c:v>
+                      <c:v>26</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5155,12 +5158,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{3ED90C93-C56E-4C17-9DC1-174B2B65BD75}</c15:txfldGUID>
+                      <c15:txfldGUID>{CF0D916C-31F1-4EC6-B0AB-8FADB25F7780}</c15:txfldGUID>
                       <c15:f>calcs!$S$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>19</c:v>
+                          <c:v>26</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5180,7 +5183,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>20</c:v>
+                      <c:v>27</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5196,12 +5199,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{FAAEAF00-E3F5-4E4C-AB48-88B679D3619B}</c15:txfldGUID>
+                      <c15:txfldGUID>{B2B175DE-4559-47A1-8EEF-687808C6B658}</c15:txfldGUID>
                       <c15:f>calcs!$T$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>20</c:v>
+                          <c:v>27</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5221,7 +5224,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>21</c:v>
+                      <c:v>28</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5237,12 +5240,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{5725D353-9DA7-474B-A702-333C49F4204F}</c15:txfldGUID>
+                      <c15:txfldGUID>{B2D41EB4-A0EF-421C-93C2-A3D842D82B66}</c15:txfldGUID>
                       <c15:f>calcs!$U$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>21</c:v>
+                          <c:v>28</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5262,7 +5265,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>22</c:v>
+                      <c:v>29</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5278,12 +5281,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{19FB9C91-AC05-4D39-9D66-5F338437ED0A}</c15:txfldGUID>
+                      <c15:txfldGUID>{6609E9DB-924C-4727-A7B6-E096615DF560}</c15:txfldGUID>
                       <c15:f>calcs!$V$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>22</c:v>
+                          <c:v>29</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5303,7 +5306,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>23</c:v>
+                      <c:v>30</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5319,12 +5322,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{C17D96D0-8D7F-4825-AD47-3E7198053CE7}</c15:txfldGUID>
+                      <c15:txfldGUID>{41923322-7AB9-42F2-8B22-79E7BF7477C1}</c15:txfldGUID>
                       <c15:f>calcs!$W$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>23</c:v>
+                          <c:v>30</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5344,7 +5347,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>24</c:v>
+                      <c:v>01</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5360,12 +5363,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{7E529747-9B3A-4522-9291-D47E782080A1}</c15:txfldGUID>
+                      <c15:txfldGUID>{F3C25235-1448-474B-8F50-30D33E7DE129}</c15:txfldGUID>
                       <c15:f>calcs!$X$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>24</c:v>
+                          <c:v>01</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5385,7 +5388,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>25</c:v>
+                      <c:v>02</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5401,12 +5404,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{24995C0F-6C84-43CA-9D57-A530D501472D}</c15:txfldGUID>
+                      <c15:txfldGUID>{7F6E0E2A-1C76-42CA-BA1D-D841B3012ECB}</c15:txfldGUID>
                       <c15:f>calcs!$Y$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>25</c:v>
+                          <c:v>02</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5426,7 +5429,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>26</c:v>
+                      <c:v>03</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5442,12 +5445,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{58E423F0-90B3-459A-8448-243FC00842FA}</c15:txfldGUID>
+                      <c15:txfldGUID>{28546F1B-B440-4CEE-90BB-004A5A3F2708}</c15:txfldGUID>
                       <c15:f>calcs!$Z$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>26</c:v>
+                          <c:v>03</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5467,7 +5470,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>27</c:v>
+                      <c:v>04</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5483,12 +5486,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{9787D0E5-0326-439B-B654-3679E41EDFAA}</c15:txfldGUID>
+                      <c15:txfldGUID>{D8F5893C-571B-4C6C-B17C-76DA709EB33D}</c15:txfldGUID>
                       <c15:f>calcs!$AA$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>27</c:v>
+                          <c:v>04</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5508,7 +5511,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>28</c:v>
+                      <c:v>05</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5524,12 +5527,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{CCDAA3CB-9146-437E-B244-B6040B6DFDCF}</c15:txfldGUID>
+                      <c15:txfldGUID>{C7274CC5-EB30-41D4-84FA-A804DBAD749B}</c15:txfldGUID>
                       <c15:f>calcs!$AB$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>28</c:v>
+                          <c:v>05</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5549,7 +5552,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>29</c:v>
+                      <c:v>06</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5565,12 +5568,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{AA1D9CEF-A365-4ADC-9D91-EF0C9CEE7442}</c15:txfldGUID>
+                      <c15:txfldGUID>{17B7FAC1-4E60-49F9-847F-EA3C0A699EC9}</c15:txfldGUID>
                       <c15:f>calcs!$AC$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>29</c:v>
+                          <c:v>06</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5590,7 +5593,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>30</c:v>
+                      <c:v>07</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5606,12 +5609,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{333C205D-53CC-4BBA-9713-76A4112A5B3F}</c15:txfldGUID>
+                      <c15:txfldGUID>{46BAB5FF-A59B-4FBC-A51E-ABCA17EA78EA}</c15:txfldGUID>
                       <c15:f>calcs!$AD$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>30</c:v>
+                          <c:v>07</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5631,7 +5634,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>01</c:v>
+                      <c:v>08</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5647,12 +5650,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{38C16B32-08BF-435D-B38E-C1863AA2430D}</c15:txfldGUID>
+                      <c15:txfldGUID>{6E1441B2-3703-4C9D-9631-A2760192CD68}</c15:txfldGUID>
                       <c15:f>calcs!$AE$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>01</c:v>
+                          <c:v>08</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5672,7 +5675,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>02</c:v>
+                      <c:v>09</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5688,12 +5691,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{29A2094D-B701-41CB-9720-69C1684DE401}</c15:txfldGUID>
+                      <c15:txfldGUID>{ABB6BBA4-2852-4BA9-BD51-BAEFE521133A}</c15:txfldGUID>
                       <c15:f>calcs!$AF$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>02</c:v>
+                          <c:v>09</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5713,7 +5716,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>03</c:v>
+                      <c:v>10</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5729,12 +5732,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{524EDC19-231D-42EE-B120-B1FC51CE47AA}</c15:txfldGUID>
+                      <c15:txfldGUID>{E11B86C3-5488-417C-995C-FD64F4C1EB5F}</c15:txfldGUID>
                       <c15:f>calcs!$AG$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>03</c:v>
+                          <c:v>10</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5754,7 +5757,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>04</c:v>
+                      <c:v>11</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5770,12 +5773,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{D2480BE9-49AA-4FFD-9CD8-27757D7B8FCD}</c15:txfldGUID>
+                      <c15:txfldGUID>{5C33A92F-6B35-4861-9CB6-946C4EFCA182}</c15:txfldGUID>
                       <c15:f>calcs!$AH$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>04</c:v>
+                          <c:v>11</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5963,7 +5966,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{7B60E4CC-C746-4A6D-9D4A-297B965E2FA7}</c15:txfldGUID>
+                      <c15:txfldGUID>{0248797B-82CB-4AD6-8ECA-672776ADAFAC}</c15:txfldGUID>
                       <c15:f>calcs!$E$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6004,7 +6007,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{0ED9359A-55A7-4A3C-9341-4655D3BA3127}</c15:txfldGUID>
+                      <c15:txfldGUID>{5A7AA0DA-E9CC-40FB-BCAF-9DF5A1980D18}</c15:txfldGUID>
                       <c15:f>calcs!$F$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6045,7 +6048,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{99B86E59-2A2F-4DF1-8D5E-329E4CE29A16}</c15:txfldGUID>
+                      <c15:txfldGUID>{58090604-CD36-4D37-93C3-06432962DA30}</c15:txfldGUID>
                       <c15:f>calcs!$G$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6086,7 +6089,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{2810ADD8-688B-4A60-BD24-38780BB930D7}</c15:txfldGUID>
+                      <c15:txfldGUID>{7884F18A-A132-40F0-8746-B8CE44EE70AD}</c15:txfldGUID>
                       <c15:f>calcs!$H$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6127,7 +6130,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{0410F87A-99D0-462A-AE5A-E3B7CE014A64}</c15:txfldGUID>
+                      <c15:txfldGUID>{24049BA6-BC64-48CD-B195-8CDBEC472BDA}</c15:txfldGUID>
                       <c15:f>calcs!$I$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6168,7 +6171,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{0D981FFC-3823-4C5F-ACF1-AB9BFFC148B3}</c15:txfldGUID>
+                      <c15:txfldGUID>{2F4E26F1-1EF4-40E1-9252-029F4050D430}</c15:txfldGUID>
                       <c15:f>calcs!$J$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6209,7 +6212,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{3A832B65-8FEB-47F7-A393-B185F1821207}</c15:txfldGUID>
+                      <c15:txfldGUID>{B17E4B90-C7AD-42D9-B1B4-1221C057F4FB}</c15:txfldGUID>
                       <c15:f>calcs!$K$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6250,7 +6253,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{3127E490-E631-4AAF-A32F-88D9171B7E58}</c15:txfldGUID>
+                      <c15:txfldGUID>{205BF8B1-7A39-44B7-A558-59C41785CA68}</c15:txfldGUID>
                       <c15:f>calcs!$L$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6291,7 +6294,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{561FF2D3-384F-4FA7-BE1B-D064C6D78290}</c15:txfldGUID>
+                      <c15:txfldGUID>{865B40D0-C7D3-494F-A9D2-F51A3A8EE773}</c15:txfldGUID>
                       <c15:f>calcs!$M$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6332,7 +6335,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{C6E1C7A4-543F-41A6-8AF1-995D62FF7FBA}</c15:txfldGUID>
+                      <c15:txfldGUID>{D8466185-2468-4E2C-A271-05EEC24BD821}</c15:txfldGUID>
                       <c15:f>calcs!$N$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6373,7 +6376,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{8AA96064-1BFD-4CFE-A623-B59FC3D149C2}</c15:txfldGUID>
+                      <c15:txfldGUID>{EDD415D8-8379-4AC3-8E68-798A225C3D01}</c15:txfldGUID>
                       <c15:f>calcs!$O$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6414,7 +6417,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{DE043912-DF88-45C5-8EC7-F3CCFDF018D5}</c15:txfldGUID>
+                      <c15:txfldGUID>{68F5EF48-F574-4640-93E7-340957257AED}</c15:txfldGUID>
                       <c15:f>calcs!$P$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6455,7 +6458,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{85202FFA-DF19-4C9E-B63C-2DB604C2B7D7}</c15:txfldGUID>
+                      <c15:txfldGUID>{21F51778-906F-4FBD-A0D2-7197B9CDF4D1}</c15:txfldGUID>
                       <c15:f>calcs!$Q$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6496,7 +6499,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{28AB5647-6935-40DC-9B63-D991997DCCA0}</c15:txfldGUID>
+                      <c15:txfldGUID>{C9250D5A-BB74-4F4D-BE3C-8C0B18A287E6}</c15:txfldGUID>
                       <c15:f>calcs!$R$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6537,7 +6540,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{C4471918-50F8-4293-8183-42C13D9D9667}</c15:txfldGUID>
+                      <c15:txfldGUID>{5EF187A7-FC6F-45D5-9159-3F8B29124DEA}</c15:txfldGUID>
                       <c15:f>calcs!$S$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6578,7 +6581,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{D1868024-139C-4CC1-B6CB-4F07A1B6FC89}</c15:txfldGUID>
+                      <c15:txfldGUID>{C5AD3F14-0D6B-41A7-8661-EB63B916464E}</c15:txfldGUID>
                       <c15:f>calcs!$T$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6619,7 +6622,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{C7190F37-4102-48E4-8338-FF35A779FDAC}</c15:txfldGUID>
+                      <c15:txfldGUID>{0EB95391-C675-49F4-8946-A5FFD3B53746}</c15:txfldGUID>
                       <c15:f>calcs!$U$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6660,7 +6663,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{A9D62DD2-974B-4E9D-BC20-54F120F8EB87}</c15:txfldGUID>
+                      <c15:txfldGUID>{C6601F5C-3663-40F8-BDBF-FE801B70FE65}</c15:txfldGUID>
                       <c15:f>calcs!$V$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6701,7 +6704,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{19D0682C-FF2E-4900-A8FF-1BFF73EE9860}</c15:txfldGUID>
+                      <c15:txfldGUID>{7B9CBE9E-4959-4CDD-951D-E36BEB92FDA5}</c15:txfldGUID>
                       <c15:f>calcs!$W$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6742,7 +6745,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{4EAD5E23-77D0-4369-9A71-ABAB48F790D9}</c15:txfldGUID>
+                      <c15:txfldGUID>{55FB2ED3-65EA-4264-A0C0-0E36106C5DF6}</c15:txfldGUID>
                       <c15:f>calcs!$X$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6783,7 +6786,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{03FEC568-7506-4B08-BE58-D01D98608A9B}</c15:txfldGUID>
+                      <c15:txfldGUID>{85C0437C-EBFF-43F9-A9E8-C565C7353E4D}</c15:txfldGUID>
                       <c15:f>calcs!$Y$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6824,7 +6827,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{70E31AFA-B687-46AC-909B-34AF2971FF8D}</c15:txfldGUID>
+                      <c15:txfldGUID>{BBF52F91-2561-46E7-8D73-D22B04A34F8B}</c15:txfldGUID>
                       <c15:f>calcs!$Z$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6865,7 +6868,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{751847D7-2DE3-4A5F-A483-D672BA3ED997}</c15:txfldGUID>
+                      <c15:txfldGUID>{D5838016-C378-4EE9-B227-C678DD24DD67}</c15:txfldGUID>
                       <c15:f>calcs!$AA$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6906,7 +6909,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{179F0E95-ADFF-4D4B-8C6B-3E57826B440C}</c15:txfldGUID>
+                      <c15:txfldGUID>{CE36BCDC-E580-48B2-895D-72509A90B131}</c15:txfldGUID>
                       <c15:f>calcs!$AB$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6947,7 +6950,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{BD47ED62-A736-49D0-8E63-BF8BD0AE920E}</c15:txfldGUID>
+                      <c15:txfldGUID>{89B2FB13-43C9-4143-8A75-46A71AB82BE6}</c15:txfldGUID>
                       <c15:f>calcs!$AC$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6988,7 +6991,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{B55C891E-F31B-4ECD-AF75-7A42C67221F9}</c15:txfldGUID>
+                      <c15:txfldGUID>{D364656A-67A2-4D87-82B5-18E9FC183E95}</c15:txfldGUID>
                       <c15:f>calcs!$AD$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -7029,7 +7032,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{448FBA0F-B234-4103-9128-DB59A3FD0522}</c15:txfldGUID>
+                      <c15:txfldGUID>{815579B5-5093-4480-95A4-C04A9D126D14}</c15:txfldGUID>
                       <c15:f>calcs!$AE$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -7070,7 +7073,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{28FBB445-9C3C-4B4A-9D27-671D11E1F944}</c15:txfldGUID>
+                      <c15:txfldGUID>{99814770-0061-4275-B3E8-DEBE89C95E86}</c15:txfldGUID>
                       <c15:f>calcs!$AF$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -7111,7 +7114,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{C123DB92-9171-4378-8397-086D6A7BA561}</c15:txfldGUID>
+                      <c15:txfldGUID>{7CC3BC65-C22C-4403-B2B8-BA5DC0C17576}</c15:txfldGUID>
                       <c15:f>calcs!$AG$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -7152,7 +7155,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{3EA59EAB-C804-437E-A830-FE75B7AEC473}</c15:txfldGUID>
+                      <c15:txfldGUID>{D3CBFA01-D10D-4F8D-BE30-80347AA0E813}</c15:txfldGUID>
                       <c15:f>calcs!$AH$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -7396,25 +7399,25 @@
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>13</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>13</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>13</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>13</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>13</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>13</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>13</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>#N/A</c:v>
@@ -7529,25 +7532,25 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>#N/A</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>#N/A</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>#N/A</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>#N/A</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>#N/A</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>#N/A</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>#N/A</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>13</c:v>
@@ -7662,7 +7665,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="16" fmlaLink="WindowOffset" horiz="1" max="500" noThreeD="1" page="7" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="16" fmlaLink="WindowOffset" horiz="1" max="500" noThreeD="1" page="7" val="7"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7731,8 +7734,8 @@
         <a:xfrm>
           <a:off x="325877" y="4038600"/>
           <a:ext cx="8988869" cy="228436"/>
-          <a:chOff x="306828" y="4108028"/>
-          <a:chExt cx="8729080" cy="223566"/>
+          <a:chOff x="306828" y="4108026"/>
+          <a:chExt cx="8729080" cy="223568"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
@@ -7806,7 +7809,7 @@
             </xdr:nvSpPr>
             <xdr:spPr bwMode="auto">
               <a:xfrm>
-                <a:off x="306828" y="4108028"/>
+                <a:off x="306828" y="4108026"/>
                 <a:ext cx="8729080" cy="163196"/>
               </a:xfrm>
               <a:prstGeom prst="rect">
@@ -7830,10 +7833,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Activities" displayName="Activities" ref="B4:F17" totalsRowShown="0">
-  <autoFilter ref="B4:F17" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C20:F25">
-    <sortCondition ref="D19:D25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Activities" displayName="Activities" ref="B4:F18" totalsRowShown="0">
+  <autoFilter ref="B4:F18" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C21:F26">
+    <sortCondition ref="D20:D26"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Id">
@@ -8088,10 +8091,10 @@
     <tabColor theme="6" tint="-0.249977111117893"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8108,22 +8111,22 @@
     <row r="1" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:7" ht="315.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
     </row>
     <row r="3" spans="1:7" s="7" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="8" t="s">
@@ -8153,7 +8156,7 @@
     <row r="5" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5">
         <f>ROW(B5)-calcs!$D$5</f>
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="C5" t="s">
         <v>22</v>
@@ -8172,7 +8175,7 @@
     <row r="6" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6">
         <f>ROW(B6)-calcs!$D$5</f>
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="C6" t="s">
         <v>23</v>
@@ -8188,7 +8191,7 @@
     <row r="7" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7">
         <f>ROW(B7)-calcs!$D$5</f>
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="C7" t="s">
         <v>24</v>
@@ -8204,7 +8207,7 @@
     <row r="8" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8">
         <f>ROW(B8)-calcs!$D$5</f>
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="C8" t="s">
         <v>25</v>
@@ -8223,7 +8226,7 @@
     <row r="9" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9">
         <f>ROW(B9)-calcs!$D$5</f>
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="C9" t="s">
         <v>29</v>
@@ -8240,7 +8243,7 @@
     <row r="10" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10">
         <f>ROW(B10)-calcs!$D$5</f>
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="C10" t="s">
         <v>28</v>
@@ -8260,7 +8263,7 @@
     <row r="11" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11">
         <f>ROW(B11)-calcs!$D$5</f>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="C11" t="s">
         <v>31</v>
@@ -8277,7 +8280,7 @@
     <row r="12" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12">
         <f>ROW(B12)-calcs!$D$5</f>
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="C12" t="s">
         <v>32</v>
@@ -8297,7 +8300,7 @@
     <row r="13" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13">
         <f>ROW(B13)-calcs!$D$5</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="C13" t="s">
         <v>36</v>
@@ -8317,7 +8320,7 @@
     <row r="14" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14">
         <f>ROW(B14)-calcs!$D$5</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" t="s">
         <v>34</v>
@@ -8337,7 +8340,7 @@
     <row r="15" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15">
         <f>ROW(B15)-calcs!$D$5</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15" t="s">
         <v>38</v>
@@ -8357,9 +8360,9 @@
     <row r="16" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16">
         <f>ROW(B16)-calcs!$D$5</f>
-        <v>3</v>
-      </c>
-      <c r="C16" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="11" t="s">
         <v>41</v>
       </c>
       <c r="D16" s="5">
@@ -8376,15 +8379,30 @@
     <row r="17" spans="2:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17">
         <f>ROW(B17)-calcs!$D$5</f>
+        <v>3</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="5">
+        <v>43804</v>
+      </c>
+      <c r="E17" s="5">
+        <v>43804</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <f>ROW(B18)-calcs!$D$5</f>
         <v>4</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D18" s="5">
         <v>43806</v>
       </c>
-      <c r="E17" s="5"/>
+      <c r="E18" s="5"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
@@ -8487,7 +8505,7 @@
       </c>
       <c r="D5">
         <f>ROWS(Activities[])</f>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -8659,7 +8677,7 @@
       </c>
       <c r="D25" s="1">
         <f>StartDate+WindowOffset</f>
-        <v>43713</v>
+        <v>43720</v>
       </c>
     </row>
     <row r="26" spans="1:35" x14ac:dyDescent="0.25">
@@ -8667,7 +8685,7 @@
         <v>3</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:35" x14ac:dyDescent="0.25">
@@ -8702,127 +8720,127 @@
       </c>
       <c r="E31" s="1">
         <f>StartDateWindow</f>
-        <v>43713</v>
+        <v>43720</v>
       </c>
       <c r="F31" s="1">
         <f t="shared" ref="F31:AI31" si="1">E31+1</f>
-        <v>43714</v>
+        <v>43721</v>
       </c>
       <c r="G31" s="1">
         <f t="shared" si="1"/>
-        <v>43715</v>
+        <v>43722</v>
       </c>
       <c r="H31" s="1">
         <f t="shared" si="1"/>
-        <v>43716</v>
+        <v>43723</v>
       </c>
       <c r="I31" s="1">
         <f t="shared" si="1"/>
-        <v>43717</v>
+        <v>43724</v>
       </c>
       <c r="J31" s="1">
         <f t="shared" si="1"/>
-        <v>43718</v>
+        <v>43725</v>
       </c>
       <c r="K31" s="1">
         <f t="shared" si="1"/>
-        <v>43719</v>
+        <v>43726</v>
       </c>
       <c r="L31" s="1">
         <f t="shared" si="1"/>
-        <v>43720</v>
+        <v>43727</v>
       </c>
       <c r="M31" s="1">
         <f t="shared" si="1"/>
-        <v>43721</v>
+        <v>43728</v>
       </c>
       <c r="N31" s="1">
         <f t="shared" si="1"/>
-        <v>43722</v>
+        <v>43729</v>
       </c>
       <c r="O31" s="1">
         <f t="shared" si="1"/>
-        <v>43723</v>
+        <v>43730</v>
       </c>
       <c r="P31" s="1">
         <f t="shared" si="1"/>
-        <v>43724</v>
+        <v>43731</v>
       </c>
       <c r="Q31" s="1">
         <f t="shared" si="1"/>
-        <v>43725</v>
+        <v>43732</v>
       </c>
       <c r="R31" s="1">
         <f t="shared" si="1"/>
-        <v>43726</v>
+        <v>43733</v>
       </c>
       <c r="S31" s="1">
         <f t="shared" si="1"/>
-        <v>43727</v>
+        <v>43734</v>
       </c>
       <c r="T31" s="1">
         <f t="shared" si="1"/>
-        <v>43728</v>
+        <v>43735</v>
       </c>
       <c r="U31" s="1">
         <f t="shared" si="1"/>
-        <v>43729</v>
+        <v>43736</v>
       </c>
       <c r="V31" s="1">
         <f t="shared" si="1"/>
-        <v>43730</v>
+        <v>43737</v>
       </c>
       <c r="W31" s="1">
         <f t="shared" si="1"/>
-        <v>43731</v>
+        <v>43738</v>
       </c>
       <c r="X31" s="1">
         <f t="shared" si="1"/>
-        <v>43732</v>
+        <v>43739</v>
       </c>
       <c r="Y31" s="1">
         <f t="shared" si="1"/>
-        <v>43733</v>
+        <v>43740</v>
       </c>
       <c r="Z31" s="1">
         <f t="shared" si="1"/>
-        <v>43734</v>
+        <v>43741</v>
       </c>
       <c r="AA31" s="1">
         <f t="shared" si="1"/>
-        <v>43735</v>
+        <v>43742</v>
       </c>
       <c r="AB31" s="1">
         <f t="shared" si="1"/>
-        <v>43736</v>
+        <v>43743</v>
       </c>
       <c r="AC31" s="1">
         <f t="shared" si="1"/>
-        <v>43737</v>
+        <v>43744</v>
       </c>
       <c r="AD31" s="1">
         <f t="shared" si="1"/>
-        <v>43738</v>
+        <v>43745</v>
       </c>
       <c r="AE31" s="1">
         <f t="shared" si="1"/>
-        <v>43739</v>
+        <v>43746</v>
       </c>
       <c r="AF31" s="1">
         <f t="shared" si="1"/>
-        <v>43740</v>
+        <v>43747</v>
       </c>
       <c r="AG31" s="1">
         <f t="shared" si="1"/>
-        <v>43741</v>
+        <v>43748</v>
       </c>
       <c r="AH31" s="1">
         <f t="shared" si="1"/>
-        <v>43742</v>
+        <v>43749</v>
       </c>
       <c r="AI31" s="1">
         <f t="shared" si="1"/>
-        <v>43743</v>
+        <v>43750</v>
       </c>
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.25">
@@ -9684,79 +9702,79 @@
       </c>
       <c r="D38" t="str">
         <f ca="1">INDEX(Activities[ACTIVITY],MATCH($C38,Activities[Id],0))</f>
-        <v>Partnering &amp; Brainstorming</v>
-      </c>
-      <c r="E38">
+        <v>LaTeX Documentation 1</v>
+      </c>
+      <c r="E38" t="e">
+        <f ca="1">GridCalc</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F38" t="e">
+        <f ca="1">GridCalc</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G38" t="e">
+        <f ca="1">GridCalc</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H38" t="e">
+        <f ca="1">GridCalc</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I38" t="e">
+        <f ca="1">GridCalc</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J38" t="e">
+        <f ca="1">GridCalc</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K38" t="e">
+        <f ca="1">GridCalc</f>
+        <v>#N/A</v>
+      </c>
+      <c r="L38" t="e">
+        <f ca="1">GridCalc</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M38" t="e">
+        <f ca="1">GridCalc</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N38" t="e">
+        <f ca="1">GridCalc</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O38">
         <f ca="1">GridCalc</f>
         <v>5.3000000000000007</v>
       </c>
-      <c r="F38">
+      <c r="P38">
         <f ca="1">GridCalc</f>
         <v>5.3000000000000007</v>
       </c>
-      <c r="G38">
+      <c r="Q38">
         <f ca="1">GridCalc</f>
         <v>5.3000000000000007</v>
       </c>
-      <c r="H38">
+      <c r="R38">
         <f ca="1">GridCalc</f>
         <v>5.3000000000000007</v>
       </c>
-      <c r="I38" t="e">
-        <f ca="1">GridCalc</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J38" t="e">
-        <f ca="1">GridCalc</f>
-        <v>#N/A</v>
-      </c>
-      <c r="K38" t="e">
-        <f ca="1">GridCalc</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L38" t="e">
-        <f ca="1">GridCalc</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M38" t="e">
-        <f ca="1">GridCalc</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N38" t="e">
-        <f ca="1">GridCalc</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O38" t="e">
-        <f ca="1">GridCalc</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P38" t="e">
-        <f ca="1">GridCalc</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Q38" t="e">
-        <f ca="1">GridCalc</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R38" t="e">
-        <f ca="1">GridCalc</f>
-        <v>#N/A</v>
-      </c>
-      <c r="S38" t="e">
-        <f ca="1">GridCalc</f>
-        <v>#N/A</v>
-      </c>
-      <c r="T38" t="e">
-        <f ca="1">GridCalc</f>
-        <v>#N/A</v>
-      </c>
-      <c r="U38" t="e">
-        <f ca="1">GridCalc</f>
-        <v>#N/A</v>
-      </c>
-      <c r="V38" t="e">
-        <f ca="1">GridCalc</f>
-        <v>#N/A</v>
+      <c r="S38">
+        <f ca="1">GridCalc</f>
+        <v>5.3000000000000007</v>
+      </c>
+      <c r="T38">
+        <f ca="1">GridCalc</f>
+        <v>5.3000000000000007</v>
+      </c>
+      <c r="U38">
+        <f ca="1">GridCalc</f>
+        <v>5.3000000000000007</v>
+      </c>
+      <c r="V38">
+        <f ca="1">GridCalc</f>
+        <v>5.3000000000000007</v>
       </c>
       <c r="W38" t="e">
         <f ca="1">GridCalc</f>
@@ -9825,7 +9843,7 @@
       </c>
       <c r="D39" t="str">
         <f ca="1">INDEX(Activities[ACTIVITY],MATCH($C39,Activities[Id],0))</f>
-        <v>LaTeX Documentation 1</v>
+        <v>Project Scope Established</v>
       </c>
       <c r="E39" t="e">
         <f ca="1">GridCalc</f>
@@ -9927,13 +9945,13 @@
         <f ca="1">GridCalc</f>
         <v>4.3000000000000007</v>
       </c>
-      <c r="AD39" t="e">
-        <f ca="1">GridCalc</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AE39" t="e">
-        <f ca="1">GridCalc</f>
-        <v>#N/A</v>
+      <c r="AD39">
+        <f ca="1">GridCalc</f>
+        <v>4.3000000000000007</v>
+      </c>
+      <c r="AE39">
+        <f ca="1">GridCalc</f>
+        <v>4.3000000000000007</v>
       </c>
       <c r="AF39" t="e">
         <f ca="1">GridCalc</f>
@@ -9966,7 +9984,7 @@
       </c>
       <c r="D40" t="str">
         <f ca="1">INDEX(Activities[ACTIVITY],MATCH($C40,Activities[Id],0))</f>
-        <v>Project Scope Established</v>
+        <v>LaTeX Documentation 2</v>
       </c>
       <c r="E40" t="e">
         <f ca="1">GridCalc</f>
@@ -10064,13 +10082,13 @@
         <f ca="1">GridCalc</f>
         <v>#N/A</v>
       </c>
-      <c r="AC40">
-        <f ca="1">GridCalc</f>
-        <v>3.3000000000000007</v>
-      </c>
-      <c r="AD40">
-        <f ca="1">GridCalc</f>
-        <v>3.3000000000000007</v>
+      <c r="AC40" t="e">
+        <f ca="1">GridCalc</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AD40" t="e">
+        <f ca="1">GridCalc</f>
+        <v>#N/A</v>
       </c>
       <c r="AE40">
         <f ca="1">GridCalc</f>
@@ -10096,123 +10114,123 @@
     <row r="43" spans="1:35" x14ac:dyDescent="0.25">
       <c r="E43" s="1">
         <f>E31</f>
-        <v>43713</v>
+        <v>43720</v>
       </c>
       <c r="F43" s="1">
         <f t="shared" ref="F43:AH43" si="4">F31</f>
-        <v>43714</v>
+        <v>43721</v>
       </c>
       <c r="G43" s="1">
         <f t="shared" si="4"/>
-        <v>43715</v>
+        <v>43722</v>
       </c>
       <c r="H43" s="1">
         <f t="shared" si="4"/>
-        <v>43716</v>
+        <v>43723</v>
       </c>
       <c r="I43" s="1">
         <f t="shared" si="4"/>
-        <v>43717</v>
+        <v>43724</v>
       </c>
       <c r="J43" s="1">
         <f t="shared" si="4"/>
-        <v>43718</v>
+        <v>43725</v>
       </c>
       <c r="K43" s="1">
         <f t="shared" si="4"/>
-        <v>43719</v>
+        <v>43726</v>
       </c>
       <c r="L43" s="1">
         <f t="shared" si="4"/>
-        <v>43720</v>
+        <v>43727</v>
       </c>
       <c r="M43" s="1">
         <f t="shared" si="4"/>
-        <v>43721</v>
+        <v>43728</v>
       </c>
       <c r="N43" s="1">
         <f t="shared" si="4"/>
-        <v>43722</v>
+        <v>43729</v>
       </c>
       <c r="O43" s="1">
         <f t="shared" si="4"/>
-        <v>43723</v>
+        <v>43730</v>
       </c>
       <c r="P43" s="1">
         <f t="shared" si="4"/>
-        <v>43724</v>
+        <v>43731</v>
       </c>
       <c r="Q43" s="1">
         <f t="shared" si="4"/>
-        <v>43725</v>
+        <v>43732</v>
       </c>
       <c r="R43" s="1">
         <f t="shared" si="4"/>
-        <v>43726</v>
+        <v>43733</v>
       </c>
       <c r="S43" s="1">
         <f t="shared" si="4"/>
-        <v>43727</v>
+        <v>43734</v>
       </c>
       <c r="T43" s="1">
         <f t="shared" si="4"/>
-        <v>43728</v>
+        <v>43735</v>
       </c>
       <c r="U43" s="1">
         <f t="shared" si="4"/>
-        <v>43729</v>
+        <v>43736</v>
       </c>
       <c r="V43" s="1">
         <f t="shared" si="4"/>
-        <v>43730</v>
+        <v>43737</v>
       </c>
       <c r="W43" s="1">
         <f t="shared" si="4"/>
-        <v>43731</v>
+        <v>43738</v>
       </c>
       <c r="X43" s="1">
         <f t="shared" si="4"/>
-        <v>43732</v>
+        <v>43739</v>
       </c>
       <c r="Y43" s="1">
         <f t="shared" si="4"/>
-        <v>43733</v>
+        <v>43740</v>
       </c>
       <c r="Z43" s="1">
         <f t="shared" si="4"/>
-        <v>43734</v>
+        <v>43741</v>
       </c>
       <c r="AA43" s="1">
         <f t="shared" si="4"/>
-        <v>43735</v>
+        <v>43742</v>
       </c>
       <c r="AB43" s="1">
         <f t="shared" si="4"/>
-        <v>43736</v>
+        <v>43743</v>
       </c>
       <c r="AC43" s="1">
         <f t="shared" si="4"/>
-        <v>43737</v>
+        <v>43744</v>
       </c>
       <c r="AD43" s="1">
         <f t="shared" si="4"/>
-        <v>43738</v>
+        <v>43745</v>
       </c>
       <c r="AE43" s="1">
         <f t="shared" si="4"/>
-        <v>43739</v>
+        <v>43746</v>
       </c>
       <c r="AF43" s="1">
         <f t="shared" si="4"/>
-        <v>43740</v>
+        <v>43747</v>
       </c>
       <c r="AG43" s="1">
         <f t="shared" si="4"/>
-        <v>43741</v>
+        <v>43748</v>
       </c>
       <c r="AH43" s="1">
         <f t="shared" si="4"/>
-        <v>43742</v>
+        <v>43749</v>
       </c>
     </row>
     <row r="44" spans="1:35" x14ac:dyDescent="0.25">
@@ -10995,14 +11013,14 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="50" spans="3:34" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:34" ht="45" x14ac:dyDescent="0.25">
       <c r="C50">
         <f t="shared" ca="1" si="6"/>
         <v>-8</v>
       </c>
       <c r="D50" t="str">
         <f ca="1">UPPER(INDEX(Activities[ACTIVITY],MATCH($C50,Activities[Id],0)))</f>
-        <v>PARTNERING &amp; BRAINSTORMING</v>
+        <v>LATEX DOCUMENTATION 1</v>
       </c>
       <c r="E50" t="e">
         <f t="shared" ref="E50:AH50" ca="1" si="12">IF(ISERROR(F38),E38,NA())</f>
@@ -11016,66 +11034,66 @@
         <f t="shared" ca="1" si="12"/>
         <v>#N/A</v>
       </c>
-      <c r="H50">
+      <c r="H50" t="e">
+        <f t="shared" ca="1" si="12"/>
+        <v>#N/A</v>
+      </c>
+      <c r="I50" t="e">
+        <f t="shared" ca="1" si="12"/>
+        <v>#N/A</v>
+      </c>
+      <c r="J50" t="e">
+        <f t="shared" ca="1" si="12"/>
+        <v>#N/A</v>
+      </c>
+      <c r="K50" t="e">
+        <f t="shared" ca="1" si="12"/>
+        <v>#N/A</v>
+      </c>
+      <c r="L50" t="e">
+        <f t="shared" ca="1" si="12"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M50" t="e">
+        <f t="shared" ca="1" si="12"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N50" t="e">
+        <f t="shared" ca="1" si="12"/>
+        <v>#N/A</v>
+      </c>
+      <c r="O50" t="e">
+        <f t="shared" ca="1" si="12"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P50" t="e">
+        <f t="shared" ca="1" si="12"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q50" t="e">
+        <f t="shared" ca="1" si="12"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R50" t="e">
+        <f t="shared" ca="1" si="12"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S50" t="e">
+        <f t="shared" ca="1" si="12"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T50" t="e">
+        <f t="shared" ca="1" si="12"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U50" t="e">
+        <f t="shared" ca="1" si="12"/>
+        <v>#N/A</v>
+      </c>
+      <c r="V50">
         <f t="shared" ca="1" si="12"/>
         <v>5.3000000000000007</v>
       </c>
-      <c r="I50" t="e">
-        <f t="shared" ca="1" si="12"/>
-        <v>#N/A</v>
-      </c>
-      <c r="J50" t="e">
-        <f t="shared" ca="1" si="12"/>
-        <v>#N/A</v>
-      </c>
-      <c r="K50" t="e">
-        <f t="shared" ca="1" si="12"/>
-        <v>#N/A</v>
-      </c>
-      <c r="L50" t="e">
-        <f t="shared" ca="1" si="12"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M50" t="e">
-        <f t="shared" ca="1" si="12"/>
-        <v>#N/A</v>
-      </c>
-      <c r="N50" t="e">
-        <f t="shared" ca="1" si="12"/>
-        <v>#N/A</v>
-      </c>
-      <c r="O50" t="e">
-        <f t="shared" ca="1" si="12"/>
-        <v>#N/A</v>
-      </c>
-      <c r="P50" t="e">
-        <f t="shared" ca="1" si="12"/>
-        <v>#N/A</v>
-      </c>
-      <c r="Q50" t="e">
-        <f t="shared" ca="1" si="12"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R50" t="e">
-        <f t="shared" ca="1" si="12"/>
-        <v>#N/A</v>
-      </c>
-      <c r="S50" t="e">
-        <f t="shared" ca="1" si="12"/>
-        <v>#N/A</v>
-      </c>
-      <c r="T50" t="e">
-        <f t="shared" ca="1" si="12"/>
-        <v>#N/A</v>
-      </c>
-      <c r="U50" t="e">
-        <f t="shared" ca="1" si="12"/>
-        <v>#N/A</v>
-      </c>
-      <c r="V50" t="e">
-        <f t="shared" ca="1" si="12"/>
-        <v>#N/A</v>
-      </c>
       <c r="W50" t="e">
         <f t="shared" ca="1" si="12"/>
         <v>#N/A</v>
@@ -11125,14 +11143,14 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="51" spans="3:34" ht="45" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:34" ht="30" x14ac:dyDescent="0.25">
       <c r="C51">
         <f t="shared" ca="1" si="6"/>
         <v>-7</v>
       </c>
       <c r="D51" t="str">
         <f ca="1">UPPER(INDEX(Activities[ACTIVITY],MATCH($C51,Activities[Id],0)))</f>
-        <v>LATEX DOCUMENTATION 1</v>
+        <v>PROJECT SCOPE ESTABLISHED</v>
       </c>
       <c r="E51" t="e">
         <f t="shared" ref="E51:AH51" ca="1" si="13">IF(ISERROR(F39),E39,NA())</f>
@@ -11230,18 +11248,18 @@
         <f t="shared" ca="1" si="13"/>
         <v>#N/A</v>
       </c>
-      <c r="AC51">
+      <c r="AC51" t="e">
+        <f t="shared" ca="1" si="13"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AD51" t="e">
+        <f t="shared" ca="1" si="13"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AE51">
         <f t="shared" ca="1" si="13"/>
         <v>4.3000000000000007</v>
       </c>
-      <c r="AD51" t="e">
-        <f t="shared" ca="1" si="13"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AE51" t="e">
-        <f t="shared" ca="1" si="13"/>
-        <v>#N/A</v>
-      </c>
       <c r="AF51" t="e">
         <f t="shared" ca="1" si="13"/>
         <v>#N/A</v>
@@ -11255,14 +11273,14 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="52" spans="3:34" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:34" ht="45" x14ac:dyDescent="0.25">
       <c r="C52">
         <f t="shared" ca="1" si="6"/>
         <v>-6</v>
       </c>
       <c r="D52" t="str">
         <f ca="1">UPPER(INDEX(Activities[ACTIVITY],MATCH($C52,Activities[Id],0)))</f>
-        <v>PROJECT SCOPE ESTABLISHED</v>
+        <v>LATEX DOCUMENTATION 2</v>
       </c>
       <c r="E52" t="e">
         <f t="shared" ref="E52:AH52" ca="1" si="14">IF(ISERROR(F40),E40,NA())</f>
@@ -11388,123 +11406,123 @@
     <row r="55" spans="3:34" x14ac:dyDescent="0.25">
       <c r="E55" s="1">
         <f>E31</f>
-        <v>43713</v>
+        <v>43720</v>
       </c>
       <c r="F55" s="1">
         <f t="shared" ref="F55:AH55" si="15">F31</f>
-        <v>43714</v>
+        <v>43721</v>
       </c>
       <c r="G55" s="1">
         <f t="shared" si="15"/>
-        <v>43715</v>
+        <v>43722</v>
       </c>
       <c r="H55" s="1">
         <f t="shared" si="15"/>
-        <v>43716</v>
+        <v>43723</v>
       </c>
       <c r="I55" s="1">
         <f t="shared" si="15"/>
-        <v>43717</v>
+        <v>43724</v>
       </c>
       <c r="J55" s="1">
         <f t="shared" si="15"/>
-        <v>43718</v>
+        <v>43725</v>
       </c>
       <c r="K55" s="1">
         <f t="shared" si="15"/>
-        <v>43719</v>
+        <v>43726</v>
       </c>
       <c r="L55" s="1">
         <f t="shared" si="15"/>
-        <v>43720</v>
+        <v>43727</v>
       </c>
       <c r="M55" s="1">
         <f t="shared" si="15"/>
-        <v>43721</v>
+        <v>43728</v>
       </c>
       <c r="N55" s="1">
         <f t="shared" si="15"/>
-        <v>43722</v>
+        <v>43729</v>
       </c>
       <c r="O55" s="1">
         <f t="shared" si="15"/>
-        <v>43723</v>
+        <v>43730</v>
       </c>
       <c r="P55" s="1">
         <f t="shared" si="15"/>
-        <v>43724</v>
+        <v>43731</v>
       </c>
       <c r="Q55" s="1">
         <f t="shared" si="15"/>
-        <v>43725</v>
+        <v>43732</v>
       </c>
       <c r="R55" s="1">
         <f t="shared" si="15"/>
-        <v>43726</v>
+        <v>43733</v>
       </c>
       <c r="S55" s="1">
         <f t="shared" si="15"/>
-        <v>43727</v>
+        <v>43734</v>
       </c>
       <c r="T55" s="1">
         <f t="shared" si="15"/>
-        <v>43728</v>
+        <v>43735</v>
       </c>
       <c r="U55" s="1">
         <f t="shared" si="15"/>
-        <v>43729</v>
+        <v>43736</v>
       </c>
       <c r="V55" s="1">
         <f t="shared" si="15"/>
-        <v>43730</v>
+        <v>43737</v>
       </c>
       <c r="W55" s="1">
         <f t="shared" si="15"/>
-        <v>43731</v>
+        <v>43738</v>
       </c>
       <c r="X55" s="1">
         <f t="shared" si="15"/>
-        <v>43732</v>
+        <v>43739</v>
       </c>
       <c r="Y55" s="1">
         <f t="shared" si="15"/>
-        <v>43733</v>
+        <v>43740</v>
       </c>
       <c r="Z55" s="1">
         <f t="shared" si="15"/>
-        <v>43734</v>
+        <v>43741</v>
       </c>
       <c r="AA55" s="1">
         <f t="shared" si="15"/>
-        <v>43735</v>
+        <v>43742</v>
       </c>
       <c r="AB55" s="1">
         <f t="shared" si="15"/>
-        <v>43736</v>
+        <v>43743</v>
       </c>
       <c r="AC55" s="1">
         <f t="shared" si="15"/>
-        <v>43737</v>
+        <v>43744</v>
       </c>
       <c r="AD55" s="1">
         <f t="shared" si="15"/>
-        <v>43738</v>
+        <v>43745</v>
       </c>
       <c r="AE55" s="1">
         <f t="shared" si="15"/>
-        <v>43739</v>
+        <v>43746</v>
       </c>
       <c r="AF55" s="1">
         <f t="shared" si="15"/>
-        <v>43740</v>
+        <v>43747</v>
       </c>
       <c r="AG55" s="1">
         <f t="shared" si="15"/>
-        <v>43741</v>
+        <v>43748</v>
       </c>
       <c r="AH55" s="1">
         <f t="shared" si="15"/>
-        <v>43742</v>
+        <v>43749</v>
       </c>
     </row>
     <row r="56" spans="3:34" x14ac:dyDescent="0.25">
@@ -11713,33 +11731,33 @@
         <f t="shared" si="17"/>
         <v>0.5</v>
       </c>
-      <c r="X58">
+      <c r="X58" t="e">
         <f t="shared" si="17"/>
-        <v>0.5</v>
-      </c>
-      <c r="Y58">
+        <v>#N/A</v>
+      </c>
+      <c r="Y58" t="e">
         <f t="shared" si="17"/>
-        <v>0.5</v>
-      </c>
-      <c r="Z58">
+        <v>#N/A</v>
+      </c>
+      <c r="Z58" t="e">
         <f t="shared" si="17"/>
-        <v>0.5</v>
-      </c>
-      <c r="AA58">
+        <v>#N/A</v>
+      </c>
+      <c r="AA58" t="e">
         <f t="shared" si="17"/>
-        <v>0.5</v>
-      </c>
-      <c r="AB58">
+        <v>#N/A</v>
+      </c>
+      <c r="AB58" t="e">
         <f t="shared" si="17"/>
-        <v>0.5</v>
-      </c>
-      <c r="AC58">
+        <v>#N/A</v>
+      </c>
+      <c r="AC58" t="e">
         <f t="shared" si="17"/>
-        <v>0.5</v>
-      </c>
-      <c r="AD58">
+        <v>#N/A</v>
+      </c>
+      <c r="AD58" t="e">
         <f t="shared" si="17"/>
-        <v>0.5</v>
+        <v>#N/A</v>
       </c>
       <c r="AE58" t="e">
         <f t="shared" si="17"/>
@@ -11839,33 +11857,33 @@
         <f t="shared" si="18"/>
         <v>13</v>
       </c>
-      <c r="X59">
+      <c r="X59" t="e">
         <f t="shared" si="18"/>
-        <v>13</v>
-      </c>
-      <c r="Y59">
+        <v>#N/A</v>
+      </c>
+      <c r="Y59" t="e">
         <f t="shared" si="18"/>
-        <v>13</v>
-      </c>
-      <c r="Z59">
+        <v>#N/A</v>
+      </c>
+      <c r="Z59" t="e">
         <f t="shared" si="18"/>
-        <v>13</v>
-      </c>
-      <c r="AA59">
+        <v>#N/A</v>
+      </c>
+      <c r="AA59" t="e">
         <f t="shared" si="18"/>
-        <v>13</v>
-      </c>
-      <c r="AB59">
+        <v>#N/A</v>
+      </c>
+      <c r="AB59" t="e">
         <f t="shared" si="18"/>
-        <v>13</v>
-      </c>
-      <c r="AC59">
+        <v>#N/A</v>
+      </c>
+      <c r="AC59" t="e">
         <f t="shared" si="18"/>
-        <v>13</v>
-      </c>
-      <c r="AD59">
+        <v>#N/A</v>
+      </c>
+      <c r="AD59" t="e">
         <f t="shared" si="18"/>
-        <v>13</v>
+        <v>#N/A</v>
       </c>
       <c r="AE59" t="e">
         <f t="shared" si="18"/>
@@ -11968,33 +11986,33 @@
         <f t="shared" si="19"/>
         <v>#N/A</v>
       </c>
-      <c r="X61" t="e">
+      <c r="X61">
         <f t="shared" si="19"/>
-        <v>#N/A</v>
-      </c>
-      <c r="Y61" t="e">
+        <v>0.5</v>
+      </c>
+      <c r="Y61">
         <f t="shared" si="19"/>
-        <v>#N/A</v>
-      </c>
-      <c r="Z61" t="e">
+        <v>0.5</v>
+      </c>
+      <c r="Z61">
         <f t="shared" si="19"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AA61" t="e">
+        <v>0.5</v>
+      </c>
+      <c r="AA61">
         <f t="shared" si="19"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AB61" t="e">
+        <v>0.5</v>
+      </c>
+      <c r="AB61">
         <f t="shared" si="19"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AC61" t="e">
+        <v>0.5</v>
+      </c>
+      <c r="AC61">
         <f t="shared" si="19"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AD61" t="e">
+        <v>0.5</v>
+      </c>
+      <c r="AD61">
         <f t="shared" si="19"/>
-        <v>#N/A</v>
+        <v>0.5</v>
       </c>
       <c r="AE61">
         <f t="shared" si="19"/>
@@ -12094,33 +12112,33 @@
         <f t="shared" si="20"/>
         <v>#N/A</v>
       </c>
-      <c r="X62" t="e">
+      <c r="X62">
         <f t="shared" si="20"/>
-        <v>#N/A</v>
-      </c>
-      <c r="Y62" t="e">
+        <v>13</v>
+      </c>
+      <c r="Y62">
         <f t="shared" si="20"/>
-        <v>#N/A</v>
-      </c>
-      <c r="Z62" t="e">
+        <v>13</v>
+      </c>
+      <c r="Z62">
         <f t="shared" si="20"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AA62" t="e">
+        <v>13</v>
+      </c>
+      <c r="AA62">
         <f t="shared" si="20"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AB62" t="e">
+        <v>13</v>
+      </c>
+      <c r="AB62">
         <f t="shared" si="20"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AC62" t="e">
+        <v>13</v>
+      </c>
+      <c r="AC62">
         <f t="shared" si="20"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AD62" t="e">
+        <v>13</v>
+      </c>
+      <c r="AD62">
         <f t="shared" si="20"/>
-        <v>#N/A</v>
+        <v>13</v>
       </c>
       <c r="AE62">
         <f t="shared" si="20"/>
@@ -12353,9 +12371,9 @@
         <f t="shared" si="21"/>
         <v>#N/A</v>
       </c>
-      <c r="Y66" t="e">
+      <c r="Y66">
         <f t="shared" si="21"/>
-        <v>#N/A</v>
+        <v>0.5</v>
       </c>
       <c r="Z66" t="e">
         <f t="shared" si="21"/>
@@ -12381,9 +12399,9 @@
         <f t="shared" si="21"/>
         <v>#N/A</v>
       </c>
-      <c r="AF66">
+      <c r="AF66" t="e">
         <f t="shared" si="21"/>
-        <v>0.5</v>
+        <v>#N/A</v>
       </c>
       <c r="AG66" t="e">
         <f t="shared" si="21"/>
@@ -12764,123 +12782,123 @@
     <row r="72" spans="4:34" x14ac:dyDescent="0.25">
       <c r="E72" t="str">
         <f>TEXT(E55,"dd")</f>
-        <v>05</v>
+        <v>12</v>
       </c>
       <c r="F72" t="str">
         <f t="shared" ref="F72:AH72" si="24">TEXT(F55,"dd")</f>
-        <v>06</v>
+        <v>13</v>
       </c>
       <c r="G72" t="str">
         <f t="shared" si="24"/>
-        <v>07</v>
+        <v>14</v>
       </c>
       <c r="H72" t="str">
         <f t="shared" si="24"/>
-        <v>08</v>
+        <v>15</v>
       </c>
       <c r="I72" t="str">
         <f t="shared" si="24"/>
-        <v>09</v>
+        <v>16</v>
       </c>
       <c r="J72" t="str">
         <f t="shared" si="24"/>
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="K72" t="str">
         <f t="shared" si="24"/>
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="L72" t="str">
         <f t="shared" si="24"/>
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="M72" t="str">
         <f t="shared" si="24"/>
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="N72" t="str">
         <f t="shared" si="24"/>
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="O72" t="str">
         <f t="shared" si="24"/>
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="P72" t="str">
         <f t="shared" si="24"/>
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="Q72" t="str">
         <f t="shared" si="24"/>
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="R72" t="str">
         <f t="shared" si="24"/>
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="S72" t="str">
         <f t="shared" si="24"/>
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="T72" t="str">
         <f t="shared" si="24"/>
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="U72" t="str">
         <f t="shared" si="24"/>
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="V72" t="str">
         <f t="shared" si="24"/>
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="W72" t="str">
         <f t="shared" si="24"/>
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="X72" t="str">
         <f t="shared" si="24"/>
-        <v>24</v>
+        <v>01</v>
       </c>
       <c r="Y72" t="str">
         <f t="shared" si="24"/>
-        <v>25</v>
+        <v>02</v>
       </c>
       <c r="Z72" t="str">
         <f t="shared" si="24"/>
-        <v>26</v>
+        <v>03</v>
       </c>
       <c r="AA72" t="str">
         <f t="shared" si="24"/>
-        <v>27</v>
+        <v>04</v>
       </c>
       <c r="AB72" t="str">
         <f t="shared" si="24"/>
-        <v>28</v>
+        <v>05</v>
       </c>
       <c r="AC72" t="str">
         <f t="shared" si="24"/>
-        <v>29</v>
+        <v>06</v>
       </c>
       <c r="AD72" t="str">
         <f t="shared" si="24"/>
-        <v>30</v>
+        <v>07</v>
       </c>
       <c r="AE72" t="str">
         <f t="shared" si="24"/>
-        <v>01</v>
+        <v>08</v>
       </c>
       <c r="AF72" t="str">
         <f t="shared" si="24"/>
-        <v>02</v>
+        <v>09</v>
       </c>
       <c r="AG72" t="str">
         <f t="shared" si="24"/>
-        <v>03</v>
+        <v>10</v>
       </c>
       <c r="AH72" t="str">
         <f t="shared" si="24"/>
-        <v>04</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -12890,23 +12908,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9677210f24a1be23c92c90fd886aa0aa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="60e05723c5c1908df1a1a4ebf11d344e" ns2:_="" ns3:_="">
     <xsd:import namespace="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
@@ -13117,25 +13118,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{983CAFE3-5C64-4732-BD1D-A9D00643597D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED11D93F-21D3-4821-9768-A0F99C41A8EB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5BB6EA-B4A9-4FD0-A581-32FE787E0D00}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13152,4 +13152,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED11D93F-21D3-4821-9768-A0F99C41A8EB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{983CAFE3-5C64-4732-BD1D-A9D00643597D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>